<commit_message>
Fix to end date for Union-Turnpike-1908, from Ken.
</commit_message>
<xml_diff>
--- a/xlsx/feature_timeline.xlsx
+++ b/xlsx/feature_timeline.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\historical-transportation-map\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D80E72-A029-4892-A205-4C0BE4311B2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3666BFEF-6B28-479A-85D2-5927A4F2F426}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2195,8 +2195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2552,7 +2552,7 @@
         <v>1809</v>
       </c>
       <c r="E18">
-        <v>9999</v>
+        <v>1965</v>
       </c>
       <c r="F18" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Fixes by Ken to names of some railroad features: 'Railroad' -> 'RR'.
</commit_message>
<xml_diff>
--- a/xlsx/feature_timeline.xlsx
+++ b/xlsx/feature_timeline.xlsx
@@ -1,27 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\historical-transportation-map\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1F9AA2-4649-4A66-BC34-F0478485B2D3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A814622-A17E-40E2-9321-F10EB6C72DEC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="feature_timeline" sheetId="1" r:id="rId1"/>
-    <sheet name="web_resources" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="379">
   <si>
     <t>layer_name</t>
   </si>
@@ -212,9 +211,6 @@
     <t>Fitchburg commuter rail line (North Station-Waltham)</t>
   </si>
   <si>
-    <t>Woburn_Branch_railroad-1844-1961</t>
-  </si>
-  <si>
     <t>Woburn Branch railroad (Wilmington-Winchester)</t>
   </si>
   <si>
@@ -224,9 +220,6 @@
     <t>Fitchburg commuter rail line (Waltham-Concord)</t>
   </si>
   <si>
-    <t>Lowell-Nashua_railroad-1844-1966</t>
-  </si>
-  <si>
     <t>Boston &amp; Maine Railroad (Lowell-Nashua)</t>
   </si>
   <si>
@@ -251,27 +244,15 @@
     <t>Old Colony railroad (Braintree-Middleborough)</t>
   </si>
   <si>
-    <t>Lowell-Lawrence_railroad-1846-1936</t>
-  </si>
-  <si>
     <t>Boston &amp; Maine Railroad (Lowell-Lawrence)</t>
   </si>
   <si>
-    <t>Hanover_Branch_railroad-1846-1941</t>
-  </si>
-  <si>
     <t>Hanover Branch railroad (Rockland-Hanover)</t>
   </si>
   <si>
-    <t>Saxonville_Branch_railroad-1846-1943</t>
-  </si>
-  <si>
     <t>Saxonville Branch railroad (Natick-Framingham)</t>
   </si>
   <si>
-    <t>Lexington_Branch_railroad-1846-1981</t>
-  </si>
-  <si>
     <t>Lexington Branch railroad (Bedford-Cambridge)</t>
   </si>
   <si>
@@ -281,63 +262,33 @@
     <t>Rockport commuter rail line (Beverly Depot-Gloucester)</t>
   </si>
   <si>
-    <t>Old_Colony_Fall_River_railroad-1847-1863</t>
-  </si>
-  <si>
     <t>Old Colony railroad (Norwood-Plainville)</t>
   </si>
   <si>
-    <t>Providence_Worcester_railroad-1847-1960</t>
-  </si>
-  <si>
     <t>Providence &amp; Worcester railroad</t>
   </si>
   <si>
-    <t>Watertown_Branch_railroad-1847-1960</t>
-  </si>
-  <si>
     <t>Watertown Branch railroad (Watertown)</t>
   </si>
   <si>
-    <t>CSX_railroad-1847-1980</t>
-  </si>
-  <si>
     <t>CSX railroad (Framingham-Milford)</t>
   </si>
   <si>
-    <t>Milford_Branch_railroad-1847-1980</t>
-  </si>
-  <si>
     <t>Milford Branch railroad (Milford)</t>
   </si>
   <si>
-    <t>Essex_railroad-1847-1985</t>
-  </si>
-  <si>
     <t>Essex railroad (Danvers-Lawrence)</t>
   </si>
   <si>
-    <t>Stoney_Brook_railroad-1848-1861</t>
-  </si>
-  <si>
     <t>Stony Brook railroad (Ayer-Lowell)</t>
   </si>
   <si>
-    <t>Milford_Secondary_railroad-1848-1972</t>
-  </si>
-  <si>
     <t>Milford Secondary railroad (Milford-Franklin)</t>
   </si>
   <si>
-    <t>Worcester-Nashua_railroad-1848-1981</t>
-  </si>
-  <si>
     <t>Worcester Nashua railroad</t>
   </si>
   <si>
-    <t>Greenville_railroad-1848-2011</t>
-  </si>
-  <si>
     <t>Boston &amp; Maine railroad (Greenville Branch)</t>
   </si>
   <si>
@@ -347,9 +298,6 @@
     <t>Franklin commuter rail line (Dedham-Franklin)</t>
   </si>
   <si>
-    <t>Manchester_Lawrence_railroad-1849-1992</t>
-  </si>
-  <si>
     <t>Manchester Lawrence railroad</t>
   </si>
   <si>
@@ -365,39 +313,21 @@
     <t>Fitchburg railroad (Marlboro-Acton)</t>
   </si>
   <si>
-    <t>Grand_Jct_railroad-1849</t>
-  </si>
-  <si>
     <t>Grand Junction (Cambridge)</t>
   </si>
   <si>
-    <t>Fitchburg_Secondary_railroad-1850</t>
-  </si>
-  <si>
     <t>Fitchburg Secondary railroad (Framingham-Fitchburg)</t>
   </si>
   <si>
-    <t>Salem-Lowell_railroad-1850-1987</t>
-  </si>
-  <si>
     <t>Salem Lowel railroad</t>
   </si>
   <si>
-    <t>Charles_River_railroad-1853-1927</t>
-  </si>
-  <si>
     <t>Charles River Line (Needham-Newton)</t>
   </si>
   <si>
-    <t>Saugus_Branch-railroad-1853-1958</t>
-  </si>
-  <si>
     <t>Saugus Branch railroad (Everett-Lynn)</t>
   </si>
   <si>
-    <t>Newburyport_railroad-1855-1981</t>
-  </si>
-  <si>
     <t>Newburyport railroad (Wakefield-Newburyport)</t>
   </si>
   <si>
@@ -422,9 +352,6 @@
     <t>Millis Branch railroad (Needham-Medway)</t>
   </si>
   <si>
-    <t>Framingham_Secondary_railroad-1867-1993</t>
-  </si>
-  <si>
     <t>Framingham Secondary railroad (Framingham-Taunton)</t>
   </si>
   <si>
@@ -434,15 +361,9 @@
     <t>Salem Turnpike (Route 107), made public highway</t>
   </si>
   <si>
-    <t>Framingham_Lowell_railroad-1871-2001</t>
-  </si>
-  <si>
     <t>Framingham Lowell railroad (Framingham-Lowell)</t>
   </si>
   <si>
-    <t>Grafton_Upton_railroad-1873-1993</t>
-  </si>
-  <si>
     <t>Grafton Upton railroad (Grafton-Milford)</t>
   </si>
   <si>
@@ -452,9 +373,6 @@
     <t>The AIR Line (Franklin-NewHaven, CT)</t>
   </si>
   <si>
-    <t>Lowell_Andover_railroad-1874-1920</t>
-  </si>
-  <si>
     <t>Lowell Andover railroad (Lowell-Andover)</t>
   </si>
   <si>
@@ -464,9 +382,6 @@
     <t>Central Massachusetts railroad (Cambridge-Northampton)</t>
   </si>
   <si>
-    <t>Lakeside_railroad-1886-1964</t>
-  </si>
-  <si>
     <t>Eastern railroad (Marblehead)</t>
   </si>
   <si>
@@ -1154,206 +1069,101 @@
     <t>y</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>url</t>
-  </si>
-  <si>
     <t>Metropolitan Transit Authority (MTA)</t>
   </si>
   <si>
-    <t>Massachusetts Bay Transporation Authority</t>
-  </si>
-  <si>
-    <t>Massachusetts Department of Transportation</t>
-  </si>
-  <si>
-    <t>https://www.mass.gov/orgs/massachusetts-department-of-transportation</t>
-  </si>
-  <si>
-    <t>https://www.mbta.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Green Line Extension </t>
-  </si>
-  <si>
-    <t>https://www.mbta.com/projects/green-line-extension-glx</t>
-  </si>
-  <si>
-    <t>https://brucefreemanrailtrail.org/</t>
-  </si>
-  <si>
-    <t>Bruce Freeman Rail Trail</t>
-  </si>
-  <si>
-    <t>https://www.mbta.com/projects/silver-line-3-chelsea-sl3</t>
-  </si>
-  <si>
-    <t>https://www.mbta.com/schedules/751/line</t>
-  </si>
-  <si>
-    <t>Sliver Line SL3 to Chelsea Project</t>
-  </si>
-  <si>
-    <t>https://www.mbta.com/schedules/743/line</t>
-  </si>
-  <si>
-    <t>https://www.mbta.com/schedules/741/line</t>
-  </si>
-  <si>
-    <t>https://www.mbta.com/schedules/742/line</t>
-  </si>
-  <si>
-    <t>Silver Line SL4 - Map and Schedule</t>
-  </si>
-  <si>
-    <t>https://www.mbta.com/schedules/749/line</t>
-  </si>
-  <si>
-    <t>Silver Line SL3 - Map and Schedule</t>
-  </si>
-  <si>
-    <t>Silver Line SL2- Map and Schedule</t>
-  </si>
-  <si>
-    <t>Silver Line SL5 - Map and Schedule</t>
-  </si>
-  <si>
-    <t>Sliver Line SL1 - Map and Schedule</t>
-  </si>
-  <si>
-    <t>Sliver Line SL2 - Map and Schedule</t>
-  </si>
-  <si>
-    <t>Silver Line SL1 - Map and Schedule</t>
-  </si>
-  <si>
-    <t>MBTA Red Line - Map and Schedule</t>
-  </si>
-  <si>
-    <t>https://www.mbta.com/schedules/Red/line</t>
-  </si>
-  <si>
-    <t>MBTA Orange Line - Map and Schedule</t>
-  </si>
-  <si>
-    <t>https://www.mbta.com/schedules/Orange/line</t>
-  </si>
-  <si>
-    <t>MBTA Blue Line - Map and Schedule</t>
-  </si>
-  <si>
-    <t>https://www.mbta.com/schedules/Blue/line</t>
-  </si>
-  <si>
     <t>Red Line (Quincy Center-Braintree)</t>
   </si>
   <si>
-    <t>Minuteman Commuter Bikeway</t>
-  </si>
-  <si>
-    <t>http://minutemanbikeway.org/</t>
-  </si>
-  <si>
-    <t>Logan Airport</t>
-  </si>
-  <si>
-    <t>http://www.massport.com/logan-airport/</t>
-  </si>
-  <si>
-    <t>https://www.mbta.com/schedules/CR-Greenbush/line</t>
-  </si>
-  <si>
-    <t>https://www.mbta.com/schedules/CR-Newburyport/line</t>
-  </si>
-  <si>
-    <t>https://www.mbta.com/schedules/CR-Kingston/line</t>
-  </si>
-  <si>
-    <t>Old Colony Commuter Rail Line (Kingston/Plymouth) - Map and Schedule</t>
-  </si>
-  <si>
-    <t>https://www.mbta.com/schedules/CR-Middleborough/line</t>
-  </si>
-  <si>
-    <t>Newburyport Commuter Rail Line - Map and Schedule</t>
-  </si>
-  <si>
-    <t>Greenbush Commuter Rail Line - Map and Schedule</t>
-  </si>
-  <si>
-    <t>Old Colony Commuter Rail Line (Middleborough/Lakeville) - Map and Schedule</t>
-  </si>
-  <si>
-    <t>Worcester Commuter Rail Line - Map and Schedule</t>
-  </si>
-  <si>
-    <t>https://www.mbta.com/schedules/CR-Fairmount/line</t>
-  </si>
-  <si>
-    <t>Fairmont Commuter Rail Line - Map and Schedule</t>
-  </si>
-  <si>
-    <t>https://www.mbta.com/schedules/CR-Worcester/timetable</t>
-  </si>
-  <si>
-    <t>https://www.mbta.com/schedules/CR-Providence/line</t>
-  </si>
-  <si>
-    <t>Stoughton Commuter Rail Line - Map and Schedule</t>
-  </si>
-  <si>
-    <t>Rockport Commuter Rail Line - Map and Schedule</t>
-  </si>
-  <si>
-    <t>Framingham Commuter Rail Line - Map and Schedule</t>
-  </si>
-  <si>
-    <t>Providence Commuter Rail Line - Map and Schedule</t>
-  </si>
-  <si>
-    <t>Lowell Commuter Rail Line - Map and Schedule</t>
-  </si>
-  <si>
-    <t>Haverhill Commuter Rail Line - Map and Schedule</t>
-  </si>
-  <si>
-    <t>Fitchburg Commuter Rail Line - Map and Schedule</t>
-  </si>
-  <si>
-    <t>Needham Commuter Rail Line - Map and Schedule</t>
-  </si>
-  <si>
-    <t>https://www.mbta.com/schedules/CR-Needham/line</t>
-  </si>
-  <si>
-    <t>https://www.mbta.com/schedules/CR-Fitchburg/timetable</t>
-  </si>
-  <si>
-    <t>https://www.mbta.com/schedules/CR-Lowell/line</t>
-  </si>
-  <si>
-    <t>https://www.mbta.com/schedules/CR-Haverhill/line</t>
-  </si>
-  <si>
-    <t>https://www.mbta.com/schedules/CR-Newburyport/timetable</t>
-  </si>
-  <si>
-    <t>Seaport-Access-2003</t>
-  </si>
-  <si>
-    <t>Seaport Access (I-90)</t>
+    <t>Woburn_Branch_RR-1844-1961</t>
+  </si>
+  <si>
+    <t>Lowell-Nashua_RR-1844-1966</t>
+  </si>
+  <si>
+    <t>Lowell-Lawrence_RR-1846-1936</t>
+  </si>
+  <si>
+    <t>Hanover_Branch_RR-1846-1941</t>
+  </si>
+  <si>
+    <t>Lexington_Branch_RR-1846-1981</t>
+  </si>
+  <si>
+    <t>Old_Colony_Fall_River_RR-1847-1863</t>
+  </si>
+  <si>
+    <t>Providence_Worcester_RR-1847-1960</t>
+  </si>
+  <si>
+    <t>Watertown_Branch_RR-1847-1960</t>
+  </si>
+  <si>
+    <t>Milford_Branch_RR-1847-1980</t>
+  </si>
+  <si>
+    <t>Stoney_Brook_RR-1848-1861</t>
+  </si>
+  <si>
+    <t>Milford_Secondary_RR-1848-1972</t>
+  </si>
+  <si>
+    <t>Worcester-Nashua_RR-1848-1981</t>
+  </si>
+  <si>
+    <t>CSX_RR-1847-1980</t>
+  </si>
+  <si>
+    <t>Saxonville_Branch_RR-1846-1943</t>
+  </si>
+  <si>
+    <t>Essex_RR-1847-1985</t>
+  </si>
+  <si>
+    <t>Greenville_RR-1848-2011</t>
+  </si>
+  <si>
+    <t>Manchester_Lawrence_RR-1849-1992</t>
+  </si>
+  <si>
+    <t>Grand_Jct_RR-1849</t>
+  </si>
+  <si>
+    <t>Charles_River_RR-1853-1927</t>
+  </si>
+  <si>
+    <t>Saugus_Branch-RR-1853-1958</t>
+  </si>
+  <si>
+    <t>Newburyport_RR-1855-1981</t>
+  </si>
+  <si>
+    <t>Salem-Lowell_RR-1850-1987</t>
+  </si>
+  <si>
+    <t>Fitchburg_Secondary_RR-1850</t>
+  </si>
+  <si>
+    <t>Framingham_Secondary_RR-1867-1993</t>
+  </si>
+  <si>
+    <t>Framingham_Lowell_RR-1871-2001</t>
+  </si>
+  <si>
+    <t>Grafton_Upton_RR-1873-1993</t>
+  </si>
+  <si>
+    <t>Lowell_Andover_RR-1874-1920</t>
+  </si>
+  <si>
+    <t>Lakeside_RR-1886-1964</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1484,14 +1294,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1794,7 +1596,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1837,14 +1639,11 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1878,7 +1677,6 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -2199,10 +1997,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F211"/>
+  <dimension ref="A1:F210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2231,7 +2029,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>375</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2767,10 +2565,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>351</v>
+      </c>
+      <c r="B35" t="s">
         <v>63</v>
-      </c>
-      <c r="B35" t="s">
-        <v>64</v>
       </c>
       <c r="C35">
         <v>1844</v>
@@ -2784,10 +2582,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" t="s">
         <v>65</v>
-      </c>
-      <c r="B36" t="s">
-        <v>66</v>
       </c>
       <c r="C36">
         <v>1844</v>
@@ -2801,10 +2599,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>67</v>
+        <v>352</v>
       </c>
       <c r="B37" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C37">
         <v>1844</v>
@@ -2818,10 +2616,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B38" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C38">
         <v>1845</v>
@@ -2835,10 +2633,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C39">
         <v>1845</v>
@@ -2852,10 +2650,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B40" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C40">
         <v>1845</v>
@@ -2872,7 +2670,7 @@
         <v>33</v>
       </c>
       <c r="B41" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C41">
         <v>1846</v>
@@ -2886,10 +2684,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>76</v>
+        <v>353</v>
       </c>
       <c r="B42" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C42">
         <v>1846</v>
@@ -2903,10 +2701,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>354</v>
       </c>
       <c r="B43" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C43">
         <v>1846</v>
@@ -2920,10 +2718,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>80</v>
+        <v>364</v>
       </c>
       <c r="B44" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C44">
         <v>1846</v>
@@ -2937,10 +2735,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>82</v>
+        <v>355</v>
       </c>
       <c r="B45" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C45">
         <v>1846</v>
@@ -2954,10 +2752,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B46" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C46">
         <v>1847</v>
@@ -2971,10 +2769,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>86</v>
+        <v>356</v>
       </c>
       <c r="B47" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C47">
         <v>1847</v>
@@ -2988,10 +2786,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>88</v>
+        <v>357</v>
       </c>
       <c r="B48" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C48">
         <v>1847</v>
@@ -3005,10 +2803,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>90</v>
+        <v>358</v>
       </c>
       <c r="B49" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C49">
         <v>1847</v>
@@ -3022,10 +2820,10 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>92</v>
+        <v>363</v>
       </c>
       <c r="B50" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="C50">
         <v>1847</v>
@@ -3039,10 +2837,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>94</v>
+        <v>359</v>
       </c>
       <c r="B51" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C51">
         <v>1847</v>
@@ -3056,10 +2854,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>96</v>
+        <v>365</v>
       </c>
       <c r="B52" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="C52">
         <v>1847</v>
@@ -3073,10 +2871,10 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>98</v>
+        <v>360</v>
       </c>
       <c r="B53" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C53">
         <v>1848</v>
@@ -3090,10 +2888,10 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>100</v>
+        <v>361</v>
       </c>
       <c r="B54" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="C54">
         <v>1848</v>
@@ -3107,10 +2905,10 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>102</v>
+        <v>362</v>
       </c>
       <c r="B55" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="C55">
         <v>1848</v>
@@ -3124,10 +2922,10 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>104</v>
+        <v>366</v>
       </c>
       <c r="B56" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="C56">
         <v>1848</v>
@@ -3141,10 +2939,10 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="B57" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="C57">
         <v>1849</v>
@@ -3158,10 +2956,10 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>108</v>
+        <v>367</v>
       </c>
       <c r="B58" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="C58">
         <v>1849</v>
@@ -3175,10 +2973,10 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="B59" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="C59">
         <v>1850</v>
@@ -3192,10 +2990,10 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="B60" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="C60">
         <v>1850</v>
@@ -3209,10 +3007,10 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>114</v>
+        <v>368</v>
       </c>
       <c r="B61" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="C61">
         <v>1850</v>
@@ -3226,10 +3024,10 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>116</v>
+        <v>373</v>
       </c>
       <c r="B62" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="C62">
         <v>1850</v>
@@ -3243,10 +3041,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>118</v>
+        <v>372</v>
       </c>
       <c r="B63" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="C63">
         <v>1850</v>
@@ -3260,10 +3058,10 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>120</v>
+        <v>369</v>
       </c>
       <c r="B64" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="C64">
         <v>1853</v>
@@ -3277,10 +3075,10 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>122</v>
+        <v>370</v>
       </c>
       <c r="B65" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="C65">
         <v>1853</v>
@@ -3294,10 +3092,10 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>124</v>
+        <v>371</v>
       </c>
       <c r="B66" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="C66">
         <v>1855</v>
@@ -3314,7 +3112,7 @@
         <v>33</v>
       </c>
       <c r="B67" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="C67">
         <v>1856</v>
@@ -3328,10 +3126,10 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="B68" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="C68">
         <v>1857</v>
@@ -3345,10 +3143,10 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="B69" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="C69">
         <v>1861</v>
@@ -3362,10 +3160,10 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="B70" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C70">
         <v>1861</v>
@@ -3379,10 +3177,10 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>133</v>
+        <v>374</v>
       </c>
       <c r="B71" t="s">
-        <v>134</v>
+        <v>110</v>
       </c>
       <c r="C71">
         <v>1867</v>
@@ -3396,10 +3194,10 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="B72" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="C72">
         <v>1868</v>
@@ -3413,10 +3211,10 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>137</v>
+        <v>375</v>
       </c>
       <c r="B73" t="s">
-        <v>138</v>
+        <v>113</v>
       </c>
       <c r="C73">
         <v>1871</v>
@@ -3430,10 +3228,10 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>139</v>
+        <v>376</v>
       </c>
       <c r="B74" t="s">
-        <v>140</v>
+        <v>114</v>
       </c>
       <c r="C74">
         <v>1873</v>
@@ -3447,10 +3245,10 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>141</v>
+        <v>115</v>
       </c>
       <c r="B75" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="C75">
         <v>1873</v>
@@ -3464,10 +3262,10 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>143</v>
+        <v>377</v>
       </c>
       <c r="B76" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="C76">
         <v>1874</v>
@@ -3481,10 +3279,10 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>145</v>
+        <v>118</v>
       </c>
       <c r="B77" t="s">
-        <v>146</v>
+        <v>119</v>
       </c>
       <c r="C77">
         <v>1875</v>
@@ -3498,10 +3296,10 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>147</v>
+        <v>378</v>
       </c>
       <c r="B78" t="s">
-        <v>148</v>
+        <v>120</v>
       </c>
       <c r="C78">
         <v>1886</v>
@@ -3515,10 +3313,10 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
       <c r="B79" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="C79">
         <v>1888</v>
@@ -3532,10 +3330,10 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="B80" t="s">
-        <v>152</v>
+        <v>124</v>
       </c>
       <c r="C80">
         <v>1889</v>
@@ -3549,10 +3347,10 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
       <c r="B81" t="s">
-        <v>154</v>
+        <v>126</v>
       </c>
       <c r="C81">
         <v>1889</v>
@@ -3569,7 +3367,7 @@
         <v>33</v>
       </c>
       <c r="B82" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
       <c r="C82">
         <v>1894</v>
@@ -3578,7 +3376,7 @@
         <v>1919</v>
       </c>
       <c r="E82" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -3586,7 +3384,7 @@
         <v>33</v>
       </c>
       <c r="B83" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
       <c r="C83">
         <v>1894</v>
@@ -3600,10 +3398,10 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="B84" t="s">
-        <v>159</v>
+        <v>131</v>
       </c>
       <c r="C84">
         <v>1897</v>
@@ -3617,10 +3415,10 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>160</v>
+        <v>132</v>
       </c>
       <c r="B85" t="s">
-        <v>161</v>
+        <v>133</v>
       </c>
       <c r="C85">
         <v>1898</v>
@@ -3637,7 +3435,7 @@
         <v>33</v>
       </c>
       <c r="B86" t="s">
-        <v>162</v>
+        <v>134</v>
       </c>
       <c r="C86">
         <v>1899</v>
@@ -3651,10 +3449,10 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>163</v>
+        <v>135</v>
       </c>
       <c r="B87" t="s">
-        <v>164</v>
+        <v>136</v>
       </c>
       <c r="C87">
         <v>1901</v>
@@ -3668,10 +3466,10 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>165</v>
+        <v>137</v>
       </c>
       <c r="B88" t="s">
-        <v>166</v>
+        <v>138</v>
       </c>
       <c r="C88">
         <v>1901</v>
@@ -3685,10 +3483,10 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>167</v>
+        <v>139</v>
       </c>
       <c r="B89" t="s">
-        <v>168</v>
+        <v>140</v>
       </c>
       <c r="C89">
         <v>1901</v>
@@ -3705,7 +3503,7 @@
         <v>33</v>
       </c>
       <c r="B90" t="s">
-        <v>169</v>
+        <v>141</v>
       </c>
       <c r="C90">
         <v>1901</v>
@@ -3719,10 +3517,10 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>170</v>
+        <v>142</v>
       </c>
       <c r="B91" t="s">
-        <v>171</v>
+        <v>143</v>
       </c>
       <c r="C91">
         <v>1904</v>
@@ -3736,10 +3534,10 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>172</v>
+        <v>144</v>
       </c>
       <c r="B92" t="s">
-        <v>173</v>
+        <v>145</v>
       </c>
       <c r="C92">
         <v>1906</v>
@@ -3753,10 +3551,10 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>174</v>
+        <v>146</v>
       </c>
       <c r="B93" t="s">
-        <v>175</v>
+        <v>147</v>
       </c>
       <c r="C93">
         <v>1907</v>
@@ -3770,10 +3568,10 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
       <c r="B94" t="s">
-        <v>177</v>
+        <v>149</v>
       </c>
       <c r="C94">
         <v>1908</v>
@@ -3787,10 +3585,10 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>178</v>
+        <v>150</v>
       </c>
       <c r="B95" t="s">
-        <v>179</v>
+        <v>151</v>
       </c>
       <c r="C95">
         <v>1912</v>
@@ -3804,10 +3602,10 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>180</v>
+        <v>152</v>
       </c>
       <c r="B96" t="s">
-        <v>181</v>
+        <v>153</v>
       </c>
       <c r="C96">
         <v>1912</v>
@@ -3824,7 +3622,7 @@
         <v>33</v>
       </c>
       <c r="B97" t="s">
-        <v>182</v>
+        <v>154</v>
       </c>
       <c r="C97">
         <v>1912</v>
@@ -3838,10 +3636,10 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>183</v>
+        <v>155</v>
       </c>
       <c r="B98" t="s">
-        <v>184</v>
+        <v>156</v>
       </c>
       <c r="C98">
         <v>1914</v>
@@ -3855,10 +3653,10 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>185</v>
+        <v>157</v>
       </c>
       <c r="B99" t="s">
-        <v>186</v>
+        <v>158</v>
       </c>
       <c r="C99">
         <v>1915</v>
@@ -3872,10 +3670,10 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
       <c r="B100" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="C100">
         <v>1916</v>
@@ -3889,10 +3687,10 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>189</v>
+        <v>161</v>
       </c>
       <c r="B101" t="s">
-        <v>190</v>
+        <v>162</v>
       </c>
       <c r="C101">
         <v>1917</v>
@@ -3906,10 +3704,10 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="B102" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="C102">
         <v>1918</v>
@@ -3926,7 +3724,7 @@
         <v>33</v>
       </c>
       <c r="B103" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="C103">
         <v>1919</v>
@@ -3935,15 +3733,15 @@
         <v>2009</v>
       </c>
       <c r="E103" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="B104" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="C104">
         <v>1919</v>
@@ -3960,7 +3758,7 @@
         <v>33</v>
       </c>
       <c r="B105" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
       <c r="C105">
         <v>1922</v>
@@ -3974,10 +3772,10 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>197</v>
+        <v>169</v>
       </c>
       <c r="B106" t="s">
-        <v>198</v>
+        <v>170</v>
       </c>
       <c r="C106">
         <v>1923</v>
@@ -3986,15 +3784,15 @@
         <v>9999</v>
       </c>
       <c r="E106" t="s">
-        <v>199</v>
+        <v>171</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>200</v>
+        <v>172</v>
       </c>
       <c r="B107" t="s">
-        <v>201</v>
+        <v>173</v>
       </c>
       <c r="C107">
         <v>1927</v>
@@ -4008,10 +3806,10 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>202</v>
+        <v>174</v>
       </c>
       <c r="B108" t="s">
-        <v>203</v>
+        <v>175</v>
       </c>
       <c r="C108">
         <v>1928</v>
@@ -4025,10 +3823,10 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>204</v>
+        <v>176</v>
       </c>
       <c r="B109" t="s">
-        <v>205</v>
+        <v>177</v>
       </c>
       <c r="C109">
         <v>1929</v>
@@ -4045,7 +3843,7 @@
         <v>33</v>
       </c>
       <c r="B110" t="s">
-        <v>206</v>
+        <v>178</v>
       </c>
       <c r="C110">
         <v>1930</v>
@@ -4059,10 +3857,10 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>207</v>
+        <v>179</v>
       </c>
       <c r="B111" t="s">
-        <v>208</v>
+        <v>180</v>
       </c>
       <c r="C111">
         <v>1934</v>
@@ -4079,7 +3877,7 @@
         <v>33</v>
       </c>
       <c r="B112" t="s">
-        <v>209</v>
+        <v>181</v>
       </c>
       <c r="C112">
         <v>1936</v>
@@ -4093,10 +3891,10 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>210</v>
+        <v>182</v>
       </c>
       <c r="B113" t="s">
-        <v>211</v>
+        <v>183</v>
       </c>
       <c r="C113">
         <v>1941</v>
@@ -4105,15 +3903,15 @@
         <v>9999</v>
       </c>
       <c r="E113" t="s">
-        <v>199</v>
+        <v>171</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>212</v>
+        <v>184</v>
       </c>
       <c r="B114" t="s">
-        <v>213</v>
+        <v>185</v>
       </c>
       <c r="C114">
         <v>1941</v>
@@ -4127,10 +3925,10 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>214</v>
+        <v>186</v>
       </c>
       <c r="B115" t="s">
-        <v>215</v>
+        <v>187</v>
       </c>
       <c r="C115">
         <v>1941</v>
@@ -4147,7 +3945,7 @@
         <v>33</v>
       </c>
       <c r="B116" t="s">
-        <v>216</v>
+        <v>188</v>
       </c>
       <c r="C116">
         <v>1943</v>
@@ -4156,7 +3954,7 @@
         <v>9999</v>
       </c>
       <c r="E116" t="s">
-        <v>199</v>
+        <v>171</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -4164,7 +3962,7 @@
         <v>33</v>
       </c>
       <c r="B117" t="s">
-        <v>380</v>
+        <v>349</v>
       </c>
       <c r="C117">
         <v>1947</v>
@@ -4178,10 +3976,10 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>217</v>
+        <v>189</v>
       </c>
       <c r="B118" t="s">
-        <v>218</v>
+        <v>190</v>
       </c>
       <c r="C118">
         <v>1950</v>
@@ -4195,10 +3993,10 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>219</v>
+        <v>191</v>
       </c>
       <c r="B119" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="C119">
         <v>1951</v>
@@ -4212,10 +4010,10 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>221</v>
+        <v>193</v>
       </c>
       <c r="B120" t="s">
-        <v>222</v>
+        <v>194</v>
       </c>
       <c r="C120">
         <v>1952</v>
@@ -4232,7 +4030,7 @@
         <v>33</v>
       </c>
       <c r="B121" t="s">
-        <v>223</v>
+        <v>195</v>
       </c>
       <c r="C121">
         <v>1952</v>
@@ -4246,10 +4044,10 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>224</v>
+        <v>196</v>
       </c>
       <c r="B122" t="s">
-        <v>225</v>
+        <v>197</v>
       </c>
       <c r="C122">
         <v>1952</v>
@@ -4263,10 +4061,10 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>226</v>
+        <v>198</v>
       </c>
       <c r="B123" t="s">
-        <v>227</v>
+        <v>199</v>
       </c>
       <c r="C123">
         <v>1954</v>
@@ -4280,10 +4078,10 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>228</v>
+        <v>200</v>
       </c>
       <c r="B124" t="s">
-        <v>229</v>
+        <v>201</v>
       </c>
       <c r="C124">
         <v>1954</v>
@@ -4297,10 +4095,10 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>230</v>
+        <v>202</v>
       </c>
       <c r="B125" t="s">
-        <v>231</v>
+        <v>203</v>
       </c>
       <c r="C125">
         <v>1954</v>
@@ -4314,10 +4112,10 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>232</v>
+        <v>204</v>
       </c>
       <c r="B126" t="s">
-        <v>233</v>
+        <v>205</v>
       </c>
       <c r="C126">
         <v>1955</v>
@@ -4334,7 +4132,7 @@
         <v>33</v>
       </c>
       <c r="B127" t="s">
-        <v>234</v>
+        <v>206</v>
       </c>
       <c r="C127">
         <v>1956</v>
@@ -4343,7 +4141,7 @@
         <v>9999</v>
       </c>
       <c r="E127" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -4351,7 +4149,7 @@
         <v>33</v>
       </c>
       <c r="B128" t="s">
-        <v>235</v>
+        <v>207</v>
       </c>
       <c r="C128">
         <v>1957</v>
@@ -4365,10 +4163,10 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>236</v>
+        <v>208</v>
       </c>
       <c r="B129" t="s">
-        <v>237</v>
+        <v>209</v>
       </c>
       <c r="C129">
         <v>1957</v>
@@ -4382,10 +4180,10 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="B130" t="s">
-        <v>239</v>
+        <v>211</v>
       </c>
       <c r="C130">
         <v>1957</v>
@@ -4399,10 +4197,10 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>240</v>
+        <v>212</v>
       </c>
       <c r="B131" t="s">
-        <v>241</v>
+        <v>213</v>
       </c>
       <c r="C131">
         <v>1958</v>
@@ -4416,10 +4214,10 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>374</v>
+        <v>346</v>
       </c>
       <c r="B132" t="s">
-        <v>242</v>
+        <v>214</v>
       </c>
       <c r="C132">
         <v>1958</v>
@@ -4433,10 +4231,10 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
       <c r="B133" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
       <c r="C133">
         <v>1958</v>
@@ -4453,7 +4251,7 @@
         <v>33</v>
       </c>
       <c r="B134" t="s">
-        <v>245</v>
+        <v>217</v>
       </c>
       <c r="C134">
         <v>1959</v>
@@ -4470,7 +4268,7 @@
         <v>33</v>
       </c>
       <c r="B135" t="s">
-        <v>246</v>
+        <v>218</v>
       </c>
       <c r="C135">
         <v>1959</v>
@@ -4484,10 +4282,10 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>247</v>
+        <v>219</v>
       </c>
       <c r="B136" t="s">
-        <v>248</v>
+        <v>220</v>
       </c>
       <c r="C136">
         <v>1959</v>
@@ -4501,10 +4299,10 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>249</v>
+        <v>221</v>
       </c>
       <c r="B137" t="s">
-        <v>250</v>
+        <v>222</v>
       </c>
       <c r="C137">
         <v>1961</v>
@@ -4518,10 +4316,10 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>251</v>
+        <v>223</v>
       </c>
       <c r="B138" t="s">
-        <v>252</v>
+        <v>224</v>
       </c>
       <c r="C138">
         <v>1962</v>
@@ -4535,10 +4333,10 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>253</v>
+        <v>225</v>
       </c>
       <c r="B139" t="s">
-        <v>254</v>
+        <v>226</v>
       </c>
       <c r="C139">
         <v>1962</v>
@@ -4552,10 +4350,10 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>255</v>
+        <v>227</v>
       </c>
       <c r="B140" t="s">
-        <v>256</v>
+        <v>228</v>
       </c>
       <c r="C140">
         <v>1962</v>
@@ -4569,10 +4367,10 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>257</v>
+        <v>229</v>
       </c>
       <c r="B141" t="s">
-        <v>258</v>
+        <v>230</v>
       </c>
       <c r="C141">
         <v>1963</v>
@@ -4586,10 +4384,10 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>259</v>
+        <v>231</v>
       </c>
       <c r="B142" t="s">
-        <v>260</v>
+        <v>232</v>
       </c>
       <c r="C142">
         <v>1964</v>
@@ -4603,10 +4401,10 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>261</v>
+        <v>233</v>
       </c>
       <c r="B143" t="s">
-        <v>262</v>
+        <v>234</v>
       </c>
       <c r="C143">
         <v>1964</v>
@@ -4623,7 +4421,7 @@
         <v>33</v>
       </c>
       <c r="B144" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
       <c r="C144">
         <v>1964</v>
@@ -4637,10 +4435,10 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="B145" t="s">
-        <v>265</v>
+        <v>237</v>
       </c>
       <c r="C145">
         <v>1965</v>
@@ -4654,10 +4452,10 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>232</v>
+        <v>204</v>
       </c>
       <c r="B146" t="s">
-        <v>266</v>
+        <v>238</v>
       </c>
       <c r="C146">
         <v>1965</v>
@@ -4671,10 +4469,10 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>267</v>
+        <v>239</v>
       </c>
       <c r="B147" t="s">
-        <v>268</v>
+        <v>240</v>
       </c>
       <c r="C147">
         <v>1965</v>
@@ -4688,10 +4486,10 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>269</v>
+        <v>241</v>
       </c>
       <c r="B148" t="s">
-        <v>270</v>
+        <v>242</v>
       </c>
       <c r="C148">
         <v>1966</v>
@@ -4705,10 +4503,10 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>271</v>
+        <v>243</v>
       </c>
       <c r="B149" t="s">
-        <v>272</v>
+        <v>244</v>
       </c>
       <c r="C149">
         <v>1969</v>
@@ -4722,10 +4520,10 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>273</v>
+        <v>245</v>
       </c>
       <c r="B150" t="s">
-        <v>274</v>
+        <v>246</v>
       </c>
       <c r="C150">
         <v>1970</v>
@@ -4739,10 +4537,10 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
       <c r="B151" t="s">
-        <v>276</v>
+        <v>248</v>
       </c>
       <c r="C151">
         <v>1971</v>
@@ -4756,10 +4554,10 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>277</v>
+        <v>249</v>
       </c>
       <c r="B152" t="s">
-        <v>278</v>
+        <v>250</v>
       </c>
       <c r="C152">
         <v>1973</v>
@@ -4776,7 +4574,7 @@
         <v>33</v>
       </c>
       <c r="B153" t="s">
-        <v>279</v>
+        <v>251</v>
       </c>
       <c r="C153">
         <v>1974</v>
@@ -4785,15 +4583,15 @@
         <v>9999</v>
       </c>
       <c r="E153" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>280</v>
+        <v>252</v>
       </c>
       <c r="B154" t="s">
-        <v>281</v>
+        <v>253</v>
       </c>
       <c r="C154">
         <v>1975</v>
@@ -4802,7 +4600,7 @@
         <v>9999</v>
       </c>
       <c r="E154" t="s">
-        <v>282</v>
+        <v>254</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -4810,7 +4608,7 @@
         <v>33</v>
       </c>
       <c r="B155" t="s">
-        <v>283</v>
+        <v>255</v>
       </c>
       <c r="C155">
         <v>1975</v>
@@ -4819,15 +4617,15 @@
         <v>9999</v>
       </c>
       <c r="E155" t="s">
-        <v>282</v>
+        <v>254</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>284</v>
+        <v>256</v>
       </c>
       <c r="B156" t="s">
-        <v>285</v>
+        <v>257</v>
       </c>
       <c r="C156">
         <v>1975</v>
@@ -4841,10 +4639,10 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>284</v>
+        <v>256</v>
       </c>
       <c r="B157" t="s">
-        <v>286</v>
+        <v>258</v>
       </c>
       <c r="C157">
         <v>1975</v>
@@ -4858,10 +4656,10 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>287</v>
+        <v>259</v>
       </c>
       <c r="B158" t="s">
-        <v>288</v>
+        <v>260</v>
       </c>
       <c r="C158">
         <v>1979</v>
@@ -4878,7 +4676,7 @@
         <v>33</v>
       </c>
       <c r="B159" t="s">
-        <v>289</v>
+        <v>261</v>
       </c>
       <c r="C159">
         <v>1979</v>
@@ -4892,10 +4690,10 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>290</v>
+        <v>262</v>
       </c>
       <c r="B160" t="s">
-        <v>409</v>
+        <v>350</v>
       </c>
       <c r="C160">
         <v>1980</v>
@@ -4909,10 +4707,10 @@
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>291</v>
+        <v>263</v>
       </c>
       <c r="B161" t="s">
-        <v>292</v>
+        <v>264</v>
       </c>
       <c r="C161">
         <v>1984</v>
@@ -4926,10 +4724,10 @@
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>293</v>
+        <v>265</v>
       </c>
       <c r="B162" t="s">
-        <v>294</v>
+        <v>266</v>
       </c>
       <c r="C162">
         <v>1985</v>
@@ -4943,10 +4741,10 @@
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>295</v>
+        <v>267</v>
       </c>
       <c r="B163" t="s">
-        <v>296</v>
+        <v>268</v>
       </c>
       <c r="C163">
         <v>1987</v>
@@ -4955,15 +4753,15 @@
         <v>9999</v>
       </c>
       <c r="E163" t="s">
-        <v>282</v>
+        <v>254</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>297</v>
+        <v>269</v>
       </c>
       <c r="B164" t="s">
-        <v>298</v>
+        <v>270</v>
       </c>
       <c r="C164">
         <v>1987</v>
@@ -4977,10 +4775,10 @@
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>299</v>
+        <v>271</v>
       </c>
       <c r="B165" t="s">
-        <v>300</v>
+        <v>272</v>
       </c>
       <c r="C165">
         <v>1992</v>
@@ -4989,15 +4787,15 @@
         <v>9999</v>
       </c>
       <c r="E165" t="s">
-        <v>282</v>
+        <v>254</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>301</v>
+        <v>273</v>
       </c>
       <c r="B166" t="s">
-        <v>302</v>
+        <v>274</v>
       </c>
       <c r="C166">
         <v>1992</v>
@@ -5006,7 +4804,7 @@
         <v>9999</v>
       </c>
       <c r="E166" t="s">
-        <v>282</v>
+        <v>254</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
@@ -5014,7 +4812,7 @@
         <v>33</v>
       </c>
       <c r="B167" t="s">
-        <v>303</v>
+        <v>275</v>
       </c>
       <c r="C167">
         <v>1993</v>
@@ -5031,7 +4829,7 @@
         <v>33</v>
       </c>
       <c r="B168" t="s">
-        <v>304</v>
+        <v>276</v>
       </c>
       <c r="C168">
         <v>1994</v>
@@ -5045,10 +4843,10 @@
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>305</v>
+        <v>277</v>
       </c>
       <c r="B169" t="s">
-        <v>306</v>
+        <v>278</v>
       </c>
       <c r="C169">
         <v>1994</v>
@@ -5065,7 +4863,7 @@
         <v>33</v>
       </c>
       <c r="B170" t="s">
-        <v>307</v>
+        <v>279</v>
       </c>
       <c r="C170">
         <v>1995</v>
@@ -5079,10 +4877,10 @@
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>308</v>
+        <v>280</v>
       </c>
       <c r="B171" t="s">
-        <v>309</v>
+        <v>281</v>
       </c>
       <c r="C171">
         <v>1995</v>
@@ -5099,7 +4897,7 @@
         <v>33</v>
       </c>
       <c r="B172" t="s">
-        <v>310</v>
+        <v>282</v>
       </c>
       <c r="C172">
         <v>1995</v>
@@ -5113,10 +4911,10 @@
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>311</v>
+        <v>283</v>
       </c>
       <c r="B173" t="s">
-        <v>312</v>
+        <v>284</v>
       </c>
       <c r="C173">
         <v>1997</v>
@@ -5128,7 +4926,7 @@
         <v>40</v>
       </c>
       <c r="F173" t="s">
-        <v>376</v>
+        <v>348</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
@@ -5136,7 +4934,7 @@
         <v>33</v>
       </c>
       <c r="B174" t="s">
-        <v>313</v>
+        <v>285</v>
       </c>
       <c r="C174">
         <v>1998</v>
@@ -5145,15 +4943,15 @@
         <v>9999</v>
       </c>
       <c r="E174" t="s">
-        <v>282</v>
+        <v>254</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>314</v>
+        <v>286</v>
       </c>
       <c r="B175" t="s">
-        <v>315</v>
+        <v>287</v>
       </c>
       <c r="C175">
         <v>1998</v>
@@ -5165,12 +4963,12 @@
         <v>40</v>
       </c>
       <c r="F175" t="s">
-        <v>376</v>
+        <v>348</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>316</v>
+        <v>288</v>
       </c>
       <c r="B176" t="s">
         <v>60</v>
@@ -5185,15 +4983,15 @@
         <v>40</v>
       </c>
       <c r="F176" t="s">
-        <v>376</v>
+        <v>348</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>317</v>
+        <v>289</v>
       </c>
       <c r="B177" t="s">
-        <v>318</v>
+        <v>290</v>
       </c>
       <c r="C177">
         <v>2002</v>
@@ -5202,7 +5000,7 @@
         <v>9999</v>
       </c>
       <c r="E177" t="s">
-        <v>282</v>
+        <v>254</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -5210,7 +5008,7 @@
         <v>33</v>
       </c>
       <c r="B178" t="s">
-        <v>319</v>
+        <v>291</v>
       </c>
       <c r="C178">
         <v>2002</v>
@@ -5224,10 +5022,10 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>320</v>
+        <v>292</v>
       </c>
       <c r="B179" t="s">
-        <v>321</v>
+        <v>293</v>
       </c>
       <c r="C179">
         <v>2002</v>
@@ -5241,10 +5039,10 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>440</v>
+        <v>294</v>
       </c>
       <c r="B180" t="s">
-        <v>441</v>
+        <v>295</v>
       </c>
       <c r="C180">
         <v>2003</v>
@@ -5253,15 +5051,15 @@
         <v>9999</v>
       </c>
       <c r="E180" t="s">
-        <v>18</v>
+        <v>254</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>322</v>
+        <v>33</v>
       </c>
       <c r="B181" t="s">
-        <v>323</v>
+        <v>296</v>
       </c>
       <c r="C181">
         <v>2003</v>
@@ -5270,15 +5068,15 @@
         <v>9999</v>
       </c>
       <c r="E181" t="s">
-        <v>282</v>
+        <v>18</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>33</v>
+        <v>297</v>
       </c>
       <c r="B182" t="s">
-        <v>324</v>
+        <v>298</v>
       </c>
       <c r="C182">
         <v>2003</v>
@@ -5287,21 +5085,21 @@
         <v>9999</v>
       </c>
       <c r="E182" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>325</v>
+        <v>33</v>
       </c>
       <c r="B183" t="s">
-        <v>326</v>
+        <v>299</v>
       </c>
       <c r="C183">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="D183">
-        <v>9999</v>
+        <v>2009</v>
       </c>
       <c r="E183" t="s">
         <v>37</v>
@@ -5309,27 +5107,27 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>33</v>
+        <v>300</v>
       </c>
       <c r="B184" t="s">
-        <v>327</v>
+        <v>301</v>
       </c>
       <c r="C184">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="D184">
-        <v>2009</v>
+        <v>9999</v>
       </c>
       <c r="E184" t="s">
-        <v>37</v>
+        <v>254</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>328</v>
+        <v>33</v>
       </c>
       <c r="B185" t="s">
-        <v>329</v>
+        <v>302</v>
       </c>
       <c r="C185">
         <v>2005</v>
@@ -5338,7 +5136,7 @@
         <v>9999</v>
       </c>
       <c r="E185" t="s">
-        <v>282</v>
+        <v>18</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
@@ -5346,7 +5144,7 @@
         <v>33</v>
       </c>
       <c r="B186" t="s">
-        <v>330</v>
+        <v>303</v>
       </c>
       <c r="C186">
         <v>2005</v>
@@ -5355,49 +5153,49 @@
         <v>9999</v>
       </c>
       <c r="E186" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>33</v>
+        <v>304</v>
       </c>
       <c r="B187" t="s">
-        <v>331</v>
+        <v>305</v>
       </c>
       <c r="C187">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="D187">
         <v>9999</v>
       </c>
       <c r="E187" t="s">
-        <v>40</v>
+        <v>254</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>332</v>
+        <v>306</v>
       </c>
       <c r="B188" t="s">
-        <v>333</v>
+        <v>307</v>
       </c>
       <c r="C188">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="D188">
         <v>9999</v>
       </c>
       <c r="E188" t="s">
-        <v>282</v>
+        <v>254</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>334</v>
+        <v>308</v>
       </c>
       <c r="B189" t="s">
-        <v>335</v>
+        <v>309</v>
       </c>
       <c r="C189">
         <v>2007</v>
@@ -5406,32 +5204,32 @@
         <v>9999</v>
       </c>
       <c r="E189" t="s">
-        <v>282</v>
+        <v>40</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>336</v>
+        <v>310</v>
       </c>
       <c r="B190" t="s">
-        <v>337</v>
+        <v>311</v>
       </c>
       <c r="C190">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="D190">
         <v>9999</v>
       </c>
       <c r="E190" t="s">
-        <v>40</v>
+        <v>254</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>338</v>
+        <v>33</v>
       </c>
       <c r="B191" t="s">
-        <v>339</v>
+        <v>312</v>
       </c>
       <c r="C191">
         <v>2008</v>
@@ -5440,32 +5238,32 @@
         <v>9999</v>
       </c>
       <c r="E191" t="s">
-        <v>282</v>
+        <v>254</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>33</v>
+        <v>313</v>
       </c>
       <c r="B192" t="s">
-        <v>340</v>
+        <v>314</v>
       </c>
       <c r="C192">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="D192">
         <v>9999</v>
       </c>
       <c r="E192" t="s">
-        <v>282</v>
+        <v>254</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>341</v>
+        <v>33</v>
       </c>
       <c r="B193" t="s">
-        <v>342</v>
+        <v>315</v>
       </c>
       <c r="C193">
         <v>2009</v>
@@ -5474,15 +5272,15 @@
         <v>9999</v>
       </c>
       <c r="E193" t="s">
-        <v>282</v>
+        <v>128</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>33</v>
+        <v>316</v>
       </c>
       <c r="B194" t="s">
-        <v>343</v>
+        <v>317</v>
       </c>
       <c r="C194">
         <v>2009</v>
@@ -5491,49 +5289,49 @@
         <v>9999</v>
       </c>
       <c r="E194" t="s">
-        <v>156</v>
+        <v>37</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>344</v>
+        <v>33</v>
       </c>
       <c r="B195" t="s">
-        <v>345</v>
+        <v>318</v>
       </c>
       <c r="C195">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="D195">
         <v>9999</v>
       </c>
       <c r="E195" t="s">
-        <v>37</v>
+        <v>254</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>33</v>
+        <v>319</v>
       </c>
       <c r="B196" t="s">
-        <v>346</v>
+        <v>320</v>
       </c>
       <c r="C196">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="D196">
         <v>9999</v>
       </c>
       <c r="E196" t="s">
-        <v>282</v>
+        <v>254</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>347</v>
+        <v>321</v>
       </c>
       <c r="B197" t="s">
-        <v>348</v>
+        <v>322</v>
       </c>
       <c r="C197">
         <v>2012</v>
@@ -5542,49 +5340,49 @@
         <v>9999</v>
       </c>
       <c r="E197" t="s">
-        <v>282</v>
+        <v>254</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>349</v>
+        <v>323</v>
       </c>
       <c r="B198" t="s">
-        <v>350</v>
+        <v>324</v>
       </c>
       <c r="C198">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="D198">
         <v>9999</v>
       </c>
       <c r="E198" t="s">
-        <v>282</v>
+        <v>254</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>351</v>
+        <v>325</v>
       </c>
       <c r="B199" t="s">
-        <v>352</v>
+        <v>326</v>
       </c>
       <c r="C199">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="D199">
         <v>9999</v>
       </c>
       <c r="E199" t="s">
-        <v>282</v>
+        <v>254</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>353</v>
+        <v>33</v>
       </c>
       <c r="B200" t="s">
-        <v>354</v>
+        <v>327</v>
       </c>
       <c r="C200">
         <v>2014</v>
@@ -5593,32 +5391,32 @@
         <v>9999</v>
       </c>
       <c r="E200" t="s">
-        <v>282</v>
+        <v>37</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>33</v>
+        <v>328</v>
       </c>
       <c r="B201" t="s">
-        <v>355</v>
+        <v>329</v>
       </c>
       <c r="C201">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="D201">
         <v>9999</v>
       </c>
       <c r="E201" t="s">
-        <v>37</v>
+        <v>254</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>356</v>
+        <v>330</v>
       </c>
       <c r="B202" t="s">
-        <v>357</v>
+        <v>331</v>
       </c>
       <c r="C202">
         <v>2015</v>
@@ -5627,15 +5425,15 @@
         <v>9999</v>
       </c>
       <c r="E202" t="s">
-        <v>282</v>
+        <v>254</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>358</v>
+        <v>332</v>
       </c>
       <c r="B203" t="s">
-        <v>359</v>
+        <v>333</v>
       </c>
       <c r="C203">
         <v>2015</v>
@@ -5644,24 +5442,24 @@
         <v>9999</v>
       </c>
       <c r="E203" t="s">
-        <v>282</v>
+        <v>254</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>360</v>
+        <v>33</v>
       </c>
       <c r="B204" t="s">
-        <v>361</v>
+        <v>334</v>
       </c>
       <c r="C204">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="D204">
         <v>9999</v>
       </c>
       <c r="E204" t="s">
-        <v>282</v>
+        <v>40</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
@@ -5669,10 +5467,10 @@
         <v>33</v>
       </c>
       <c r="B205" t="s">
-        <v>362</v>
+        <v>335</v>
       </c>
       <c r="C205">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="D205">
         <v>9999</v>
@@ -5683,27 +5481,27 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>33</v>
+        <v>336</v>
       </c>
       <c r="B206" t="s">
-        <v>363</v>
+        <v>337</v>
       </c>
       <c r="C206">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="D206">
         <v>9999</v>
       </c>
       <c r="E206" t="s">
-        <v>40</v>
+        <v>254</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>364</v>
+        <v>338</v>
       </c>
       <c r="B207" t="s">
-        <v>365</v>
+        <v>339</v>
       </c>
       <c r="C207">
         <v>2018</v>
@@ -5712,15 +5510,15 @@
         <v>9999</v>
       </c>
       <c r="E207" t="s">
-        <v>282</v>
+        <v>254</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>366</v>
+        <v>340</v>
       </c>
       <c r="B208" t="s">
-        <v>367</v>
+        <v>341</v>
       </c>
       <c r="C208">
         <v>2018</v>
@@ -5729,804 +5527,44 @@
         <v>9999</v>
       </c>
       <c r="E208" t="s">
-        <v>282</v>
+        <v>37</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>368</v>
+        <v>342</v>
       </c>
       <c r="B209" t="s">
-        <v>369</v>
+        <v>343</v>
       </c>
       <c r="C209">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="D209">
         <v>9999</v>
       </c>
       <c r="E209" t="s">
-        <v>37</v>
+        <v>254</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>370</v>
+        <v>344</v>
       </c>
       <c r="B210" t="s">
-        <v>371</v>
+        <v>345</v>
       </c>
       <c r="C210">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="D210">
         <v>9999</v>
       </c>
       <c r="E210" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
-        <v>372</v>
-      </c>
-      <c r="B211" t="s">
-        <v>373</v>
-      </c>
-      <c r="C211">
-        <v>2021</v>
-      </c>
-      <c r="D211">
-        <v>9999</v>
-      </c>
-      <c r="E211" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD2C86BE-75AB-4E87-B5FA-FBF3BC510317}">
-  <dimension ref="A1:C60"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="71.7109375" customWidth="1"/>
-    <col min="3" max="3" width="90.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>377</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>432</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B16" t="s">
-        <v>405</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B17" t="s">
-        <v>405</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B18" t="s">
-        <v>407</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B19" t="s">
-        <v>434</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B20" t="s">
-        <v>434</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B21" t="s">
-        <v>405</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B22" t="s">
-        <v>403</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B23" t="s">
-        <v>403</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B24" t="s">
-        <v>407</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B25" t="s">
-        <v>403</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B26" t="s">
-        <v>403</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B27" t="s">
-        <v>405</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B28" t="s">
-        <v>412</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B29" t="s">
-        <v>403</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B30" t="s">
-        <v>403</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B31" t="s">
-        <v>403</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B32" t="s">
-        <v>407</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B33" t="s">
-        <v>407</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B34" t="s">
-        <v>381</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B35" t="s">
-        <v>403</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B36" t="s">
-        <v>405</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B37" t="s">
-        <v>405</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B38" t="s">
-        <v>424</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B39" t="s">
-        <v>403</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B40" t="s">
-        <v>403</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B41" t="s">
-        <v>403</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B42" t="s">
-        <v>405</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B43" t="s">
-        <v>410</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B44" t="s">
-        <v>422</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B45" t="s">
-        <v>417</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B46" t="s">
-        <v>421</v>
-      </c>
-      <c r="C46" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B47" t="s">
-        <v>419</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B48" t="s">
-        <v>395</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B49" t="s">
-        <v>399</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B50" t="s">
-        <v>402</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B51" t="s">
-        <v>398</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B52" t="s">
-        <v>420</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B53" t="s">
-        <v>388</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B54" t="s">
-        <v>382</v>
-      </c>
-      <c r="C54" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B55" t="s">
-        <v>400</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B56" t="s">
-        <v>401</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B57" t="s">
-        <v>388</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B58" t="s">
-        <v>391</v>
-      </c>
-      <c r="C58" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B59" t="s">
-        <v>397</v>
-      </c>
-      <c r="C59" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="e">
-        <f>feature_timeline!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B60" t="s">
-        <v>385</v>
-      </c>
-      <c r="C60" t="s">
-        <v>386</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C34" r:id="rId1" xr:uid="{9044FEFB-5CC1-44E8-9FDC-E8325A98748A}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Restored Seaport-Access-2003, inadvertently deleted in previous version.
</commit_message>
<xml_diff>
--- a/xlsx/feature_timeline.xlsx
+++ b/xlsx/feature_timeline.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\historical-transportation-map\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A814622-A17E-40E2-9321-F10EB6C72DEC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB554952-AE32-4DD7-B942-B6A8A8877342}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="381">
   <si>
     <t>layer_name</t>
   </si>
@@ -1157,6 +1157,12 @@
   </si>
   <si>
     <t>Lakeside_RR-1886-1964</t>
+  </si>
+  <si>
+    <t>Seaport-Access-2003</t>
+  </si>
+  <si>
+    <t>Seaport Access</t>
   </si>
 </sst>
 </file>
@@ -1997,10 +2003,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F210"/>
+  <dimension ref="A1:F211"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A172" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E179" sqref="E179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5022,44 +5028,44 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>292</v>
+        <v>379</v>
       </c>
       <c r="B179" t="s">
-        <v>293</v>
+        <v>380</v>
       </c>
       <c r="C179">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="D179">
         <v>9999</v>
       </c>
       <c r="E179" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B180" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C180">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="D180">
         <v>9999</v>
       </c>
       <c r="E180" t="s">
-        <v>254</v>
+        <v>37</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>33</v>
+        <v>294</v>
       </c>
       <c r="B181" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C181">
         <v>2003</v>
@@ -5068,15 +5074,15 @@
         <v>9999</v>
       </c>
       <c r="E181" t="s">
-        <v>18</v>
+        <v>254</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>297</v>
+        <v>33</v>
       </c>
       <c r="B182" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C182">
         <v>2003</v>
@@ -5085,21 +5091,21 @@
         <v>9999</v>
       </c>
       <c r="E182" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>33</v>
+        <v>297</v>
       </c>
       <c r="B183" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C183">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D183">
-        <v>2009</v>
+        <v>9999</v>
       </c>
       <c r="E183" t="s">
         <v>37</v>
@@ -5107,27 +5113,27 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>300</v>
+        <v>33</v>
       </c>
       <c r="B184" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C184">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="D184">
-        <v>9999</v>
+        <v>2009</v>
       </c>
       <c r="E184" t="s">
-        <v>254</v>
+        <v>37</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>33</v>
+        <v>300</v>
       </c>
       <c r="B185" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C185">
         <v>2005</v>
@@ -5136,7 +5142,7 @@
         <v>9999</v>
       </c>
       <c r="E185" t="s">
-        <v>18</v>
+        <v>254</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
@@ -5144,7 +5150,7 @@
         <v>33</v>
       </c>
       <c r="B186" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C186">
         <v>2005</v>
@@ -5153,35 +5159,35 @@
         <v>9999</v>
       </c>
       <c r="E186" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>304</v>
+        <v>33</v>
       </c>
       <c r="B187" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C187">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="D187">
         <v>9999</v>
       </c>
       <c r="E187" t="s">
-        <v>254</v>
+        <v>40</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B188" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C188">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="D188">
         <v>9999</v>
@@ -5192,10 +5198,10 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B189" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C189">
         <v>2007</v>
@@ -5204,32 +5210,32 @@
         <v>9999</v>
       </c>
       <c r="E189" t="s">
-        <v>40</v>
+        <v>254</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B190" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C190">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="D190">
         <v>9999</v>
       </c>
       <c r="E190" t="s">
-        <v>254</v>
+        <v>40</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>33</v>
+        <v>310</v>
       </c>
       <c r="B191" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C191">
         <v>2008</v>
@@ -5243,13 +5249,13 @@
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>313</v>
+        <v>33</v>
       </c>
       <c r="B192" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C192">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="D192">
         <v>9999</v>
@@ -5260,10 +5266,10 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>33</v>
+        <v>313</v>
       </c>
       <c r="B193" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C193">
         <v>2009</v>
@@ -5272,15 +5278,15 @@
         <v>9999</v>
       </c>
       <c r="E193" t="s">
-        <v>128</v>
+        <v>254</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>316</v>
+        <v>33</v>
       </c>
       <c r="B194" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C194">
         <v>2009</v>
@@ -5289,35 +5295,35 @@
         <v>9999</v>
       </c>
       <c r="E194" t="s">
-        <v>37</v>
+        <v>128</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>33</v>
+        <v>316</v>
       </c>
       <c r="B195" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C195">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="D195">
         <v>9999</v>
       </c>
       <c r="E195" t="s">
-        <v>254</v>
+        <v>37</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>319</v>
+        <v>33</v>
       </c>
       <c r="B196" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C196">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="D196">
         <v>9999</v>
@@ -5328,10 +5334,10 @@
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B197" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C197">
         <v>2012</v>
@@ -5345,13 +5351,13 @@
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B198" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C198">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="D198">
         <v>9999</v>
@@ -5362,13 +5368,13 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B199" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C199">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D199">
         <v>9999</v>
@@ -5379,10 +5385,10 @@
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>33</v>
+        <v>325</v>
       </c>
       <c r="B200" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C200">
         <v>2014</v>
@@ -5391,32 +5397,32 @@
         <v>9999</v>
       </c>
       <c r="E200" t="s">
-        <v>37</v>
+        <v>254</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>328</v>
+        <v>33</v>
       </c>
       <c r="B201" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C201">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D201">
         <v>9999</v>
       </c>
       <c r="E201" t="s">
-        <v>254</v>
+        <v>37</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B202" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C202">
         <v>2015</v>
@@ -5430,10 +5436,10 @@
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B203" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C203">
         <v>2015</v>
@@ -5447,19 +5453,19 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>33</v>
+        <v>332</v>
       </c>
       <c r="B204" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C204">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D204">
         <v>9999</v>
       </c>
       <c r="E204" t="s">
-        <v>40</v>
+        <v>254</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
@@ -5467,10 +5473,10 @@
         <v>33</v>
       </c>
       <c r="B205" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C205">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="D205">
         <v>9999</v>
@@ -5481,27 +5487,27 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>336</v>
+        <v>33</v>
       </c>
       <c r="B206" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C206">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="D206">
         <v>9999</v>
       </c>
       <c r="E206" t="s">
-        <v>254</v>
+        <v>40</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B207" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C207">
         <v>2018</v>
@@ -5515,10 +5521,10 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B208" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C208">
         <v>2018</v>
@@ -5527,40 +5533,57 @@
         <v>9999</v>
       </c>
       <c r="E208" t="s">
-        <v>37</v>
+        <v>254</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B209" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C209">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D209">
         <v>9999</v>
       </c>
       <c r="E209" t="s">
-        <v>254</v>
+        <v>37</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
+        <v>342</v>
+      </c>
+      <c r="B210" t="s">
+        <v>343</v>
+      </c>
+      <c r="C210">
+        <v>2019</v>
+      </c>
+      <c r="D210">
+        <v>9999</v>
+      </c>
+      <c r="E210" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
         <v>344</v>
       </c>
-      <c r="B210" t="s">
+      <c r="B211" t="s">
         <v>345</v>
       </c>
-      <c r="C210">
+      <c r="C211">
         <v>2021</v>
       </c>
-      <c r="D210">
-        <v>9999</v>
-      </c>
-      <c r="E210" t="s">
+      <c r="D211">
+        <v>9999</v>
+      </c>
+      <c r="E211" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corrected entry for 'Seaport Access Road'.
</commit_message>
<xml_diff>
--- a/xlsx/feature_timeline.xlsx
+++ b/xlsx/feature_timeline.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\historical-transportation-map\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB554952-AE32-4DD7-B942-B6A8A8877342}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D9A09C-F892-4832-A2AB-AC8E040C5CA0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1162,7 +1162,7 @@
     <t>Seaport-Access-2003</t>
   </si>
   <si>
-    <t>Seaport Access</t>
+    <t>Seaport Access Road</t>
   </si>
 </sst>
 </file>
@@ -2005,8 +2005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E179" sqref="E179"/>
+    <sheetView tabSelected="1" topLeftCell="A178" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B179" sqref="B179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated spreadsheets (including changes to 2 SVG layer names) based on feedback from Jonathan Belcher, and discussion with Ken 5/13/21.
</commit_message>
<xml_diff>
--- a/xlsx/feature_timeline.xlsx
+++ b/xlsx/feature_timeline.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\historical-transportation-map\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D9A09C-F892-4832-A2AB-AC8E040C5CA0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B834CB-237D-473D-A7D3-462261C34EA2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -466,9 +466,6 @@
     <t>Needham commuter rail line (Needham Junction-Needham Heights)</t>
   </si>
   <si>
-    <t>Orange_Line-1908-1987</t>
-  </si>
-  <si>
     <t>Orange Line (Dudley-Forest Hills)</t>
   </si>
   <si>
@@ -505,9 +502,6 @@
     <t>Blue Line (Government Center-Bowdoin)</t>
   </si>
   <si>
-    <t>Red_Line-1917</t>
-  </si>
-  <si>
     <t>Red Line (Downtown commuter rail crossing-South Station)</t>
   </si>
   <si>
@@ -583,9 +577,6 @@
     <t>Green_Line_Huntington-1941-1985</t>
   </si>
   <si>
-    <t>Green Line Arborway (E Line)</t>
-  </si>
-  <si>
     <t>Boston Airport renamed Logan Airport</t>
   </si>
   <si>
@@ -913,9 +904,6 @@
     <t>Depressed I-93 North and I-90 Connector</t>
   </si>
   <si>
-    <t>SilverLine-Waterfront-2003</t>
-  </si>
-  <si>
     <t>Silver Line Waterfront</t>
   </si>
   <si>
@@ -1163,6 +1151,18 @@
   </si>
   <si>
     <t>Seaport Access Road</t>
+  </si>
+  <si>
+    <t>Orange_Line-1909-1987</t>
+  </si>
+  <si>
+    <t>SilverLine-Waterfront-2004</t>
+  </si>
+  <si>
+    <t>Red_Line-1916</t>
+  </si>
+  <si>
+    <t>Green Line (E Line) cut back from Arborway to Heath</t>
   </si>
 </sst>
 </file>
@@ -2005,8 +2005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B179" sqref="B179"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2035,7 +2035,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2571,7 +2571,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B35" t="s">
         <v>63</v>
@@ -2605,7 +2605,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B37" t="s">
         <v>66</v>
@@ -2690,7 +2690,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="B42" t="s">
         <v>74</v>
@@ -2707,7 +2707,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B43" t="s">
         <v>75</v>
@@ -2724,7 +2724,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="B44" t="s">
         <v>76</v>
@@ -2741,7 +2741,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B45" t="s">
         <v>77</v>
@@ -2775,7 +2775,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B47" t="s">
         <v>80</v>
@@ -2792,7 +2792,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B48" t="s">
         <v>81</v>
@@ -2809,7 +2809,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B49" t="s">
         <v>82</v>
@@ -2826,7 +2826,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B50" t="s">
         <v>83</v>
@@ -2843,7 +2843,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B51" t="s">
         <v>84</v>
@@ -2860,7 +2860,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="B52" t="s">
         <v>85</v>
@@ -2877,7 +2877,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B53" t="s">
         <v>86</v>
@@ -2894,7 +2894,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B54" t="s">
         <v>87</v>
@@ -2911,7 +2911,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="B55" t="s">
         <v>88</v>
@@ -2928,7 +2928,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B56" t="s">
         <v>89</v>
@@ -2962,7 +2962,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B58" t="s">
         <v>92</v>
@@ -3013,7 +3013,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B61" t="s">
         <v>97</v>
@@ -3030,7 +3030,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B62" t="s">
         <v>98</v>
@@ -3047,7 +3047,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="B63" t="s">
         <v>99</v>
@@ -3064,7 +3064,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="B64" t="s">
         <v>100</v>
@@ -3081,7 +3081,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="B65" t="s">
         <v>101</v>
@@ -3098,7 +3098,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B66" t="s">
         <v>102</v>
@@ -3183,7 +3183,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B71" t="s">
         <v>110</v>
@@ -3217,7 +3217,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B73" t="s">
         <v>113</v>
@@ -3234,7 +3234,7 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="B74" t="s">
         <v>114</v>
@@ -3268,7 +3268,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B76" t="s">
         <v>117</v>
@@ -3302,7 +3302,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="B78" t="s">
         <v>120</v>
@@ -3574,13 +3574,13 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>377</v>
+      </c>
+      <c r="B94" t="s">
         <v>148</v>
       </c>
-      <c r="B94" t="s">
-        <v>149</v>
-      </c>
       <c r="C94">
-        <v>1908</v>
+        <v>1909</v>
       </c>
       <c r="D94">
         <v>1987</v>
@@ -3591,10 +3591,10 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>149</v>
+      </c>
+      <c r="B95" t="s">
         <v>150</v>
-      </c>
-      <c r="B95" t="s">
-        <v>151</v>
       </c>
       <c r="C95">
         <v>1912</v>
@@ -3608,10 +3608,10 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
+        <v>151</v>
+      </c>
+      <c r="B96" t="s">
         <v>152</v>
-      </c>
-      <c r="B96" t="s">
-        <v>153</v>
       </c>
       <c r="C96">
         <v>1912</v>
@@ -3628,7 +3628,7 @@
         <v>33</v>
       </c>
       <c r="B97" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C97">
         <v>1912</v>
@@ -3642,10 +3642,10 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
+        <v>154</v>
+      </c>
+      <c r="B98" t="s">
         <v>155</v>
-      </c>
-      <c r="B98" t="s">
-        <v>156</v>
       </c>
       <c r="C98">
         <v>1914</v>
@@ -3659,10 +3659,10 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>156</v>
+      </c>
+      <c r="B99" t="s">
         <v>157</v>
-      </c>
-      <c r="B99" t="s">
-        <v>158</v>
       </c>
       <c r="C99">
         <v>1915</v>
@@ -3676,10 +3676,10 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>158</v>
+      </c>
+      <c r="B100" t="s">
         <v>159</v>
-      </c>
-      <c r="B100" t="s">
-        <v>160</v>
       </c>
       <c r="C100">
         <v>1916</v>
@@ -3693,13 +3693,13 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>161</v>
+        <v>379</v>
       </c>
       <c r="B101" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C101">
-        <v>1917</v>
+        <v>1916</v>
       </c>
       <c r="D101">
         <v>9999</v>
@@ -3710,10 +3710,10 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B102" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C102">
         <v>1918</v>
@@ -3730,7 +3730,7 @@
         <v>33</v>
       </c>
       <c r="B103" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C103">
         <v>1919</v>
@@ -3744,10 +3744,10 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B104" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C104">
         <v>1919</v>
@@ -3764,7 +3764,7 @@
         <v>33</v>
       </c>
       <c r="B105" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C105">
         <v>1922</v>
@@ -3778,10 +3778,10 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B106" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C106">
         <v>1923</v>
@@ -3790,15 +3790,15 @@
         <v>9999</v>
       </c>
       <c r="E106" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B107" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C107">
         <v>1927</v>
@@ -3812,10 +3812,10 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B108" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C108">
         <v>1928</v>
@@ -3829,10 +3829,10 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B109" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C109">
         <v>1929</v>
@@ -3849,7 +3849,7 @@
         <v>33</v>
       </c>
       <c r="B110" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C110">
         <v>1930</v>
@@ -3863,10 +3863,10 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B111" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C111">
         <v>1934</v>
@@ -3883,7 +3883,7 @@
         <v>33</v>
       </c>
       <c r="B112" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C112">
         <v>1936</v>
@@ -3897,10 +3897,10 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B113" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C113">
         <v>1941</v>
@@ -3909,15 +3909,15 @@
         <v>9999</v>
       </c>
       <c r="E113" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B114" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C114">
         <v>1941</v>
@@ -3931,10 +3931,10 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B115" t="s">
-        <v>187</v>
+        <v>380</v>
       </c>
       <c r="C115">
         <v>1941</v>
@@ -3951,7 +3951,7 @@
         <v>33</v>
       </c>
       <c r="B116" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C116">
         <v>1943</v>
@@ -3960,7 +3960,7 @@
         <v>9999</v>
       </c>
       <c r="E116" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -3968,7 +3968,7 @@
         <v>33</v>
       </c>
       <c r="B117" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="C117">
         <v>1947</v>
@@ -3982,10 +3982,10 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B118" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C118">
         <v>1950</v>
@@ -3999,10 +3999,10 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B119" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C119">
         <v>1951</v>
@@ -4016,10 +4016,10 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B120" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C120">
         <v>1952</v>
@@ -4036,7 +4036,7 @@
         <v>33</v>
       </c>
       <c r="B121" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C121">
         <v>1952</v>
@@ -4050,10 +4050,10 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B122" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C122">
         <v>1952</v>
@@ -4067,10 +4067,10 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B123" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C123">
         <v>1954</v>
@@ -4084,10 +4084,10 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B124" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C124">
         <v>1954</v>
@@ -4101,10 +4101,10 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B125" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C125">
         <v>1954</v>
@@ -4118,10 +4118,10 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B126" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C126">
         <v>1955</v>
@@ -4138,7 +4138,7 @@
         <v>33</v>
       </c>
       <c r="B127" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C127">
         <v>1956</v>
@@ -4155,7 +4155,7 @@
         <v>33</v>
       </c>
       <c r="B128" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C128">
         <v>1957</v>
@@ -4169,10 +4169,10 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B129" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C129">
         <v>1957</v>
@@ -4186,10 +4186,10 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B130" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C130">
         <v>1957</v>
@@ -4203,10 +4203,10 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B131" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C131">
         <v>1958</v>
@@ -4220,10 +4220,10 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B132" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C132">
         <v>1958</v>
@@ -4237,10 +4237,10 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B133" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C133">
         <v>1958</v>
@@ -4257,7 +4257,7 @@
         <v>33</v>
       </c>
       <c r="B134" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C134">
         <v>1959</v>
@@ -4274,7 +4274,7 @@
         <v>33</v>
       </c>
       <c r="B135" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C135">
         <v>1959</v>
@@ -4288,10 +4288,10 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B136" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C136">
         <v>1959</v>
@@ -4305,10 +4305,10 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B137" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C137">
         <v>1961</v>
@@ -4322,10 +4322,10 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B138" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C138">
         <v>1962</v>
@@ -4339,10 +4339,10 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B139" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C139">
         <v>1962</v>
@@ -4356,10 +4356,10 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B140" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C140">
         <v>1962</v>
@@ -4373,10 +4373,10 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B141" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C141">
         <v>1963</v>
@@ -4390,10 +4390,10 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B142" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C142">
         <v>1964</v>
@@ -4407,10 +4407,10 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B143" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C143">
         <v>1964</v>
@@ -4427,7 +4427,7 @@
         <v>33</v>
       </c>
       <c r="B144" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C144">
         <v>1964</v>
@@ -4441,10 +4441,10 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B145" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C145">
         <v>1965</v>
@@ -4458,10 +4458,10 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B146" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C146">
         <v>1965</v>
@@ -4475,10 +4475,10 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B147" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C147">
         <v>1965</v>
@@ -4492,10 +4492,10 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B148" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C148">
         <v>1966</v>
@@ -4509,10 +4509,10 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B149" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C149">
         <v>1969</v>
@@ -4526,10 +4526,10 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B150" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C150">
         <v>1970</v>
@@ -4543,10 +4543,10 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B151" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C151">
         <v>1971</v>
@@ -4560,10 +4560,10 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B152" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C152">
         <v>1973</v>
@@ -4580,7 +4580,7 @@
         <v>33</v>
       </c>
       <c r="B153" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C153">
         <v>1974</v>
@@ -4594,10 +4594,10 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B154" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C154">
         <v>1975</v>
@@ -4606,7 +4606,7 @@
         <v>9999</v>
       </c>
       <c r="E154" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -4614,7 +4614,7 @@
         <v>33</v>
       </c>
       <c r="B155" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C155">
         <v>1975</v>
@@ -4623,15 +4623,15 @@
         <v>9999</v>
       </c>
       <c r="E155" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B156" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C156">
         <v>1975</v>
@@ -4645,10 +4645,10 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B157" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C157">
         <v>1975</v>
@@ -4662,10 +4662,10 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B158" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C158">
         <v>1979</v>
@@ -4682,7 +4682,7 @@
         <v>33</v>
       </c>
       <c r="B159" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C159">
         <v>1979</v>
@@ -4696,10 +4696,10 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B160" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C160">
         <v>1980</v>
@@ -4713,10 +4713,10 @@
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B161" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C161">
         <v>1984</v>
@@ -4730,10 +4730,10 @@
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B162" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C162">
         <v>1985</v>
@@ -4747,10 +4747,10 @@
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B163" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C163">
         <v>1987</v>
@@ -4759,15 +4759,15 @@
         <v>9999</v>
       </c>
       <c r="E163" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B164" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C164">
         <v>1987</v>
@@ -4781,10 +4781,10 @@
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B165" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C165">
         <v>1992</v>
@@ -4793,15 +4793,15 @@
         <v>9999</v>
       </c>
       <c r="E165" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B166" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C166">
         <v>1992</v>
@@ -4810,7 +4810,7 @@
         <v>9999</v>
       </c>
       <c r="E166" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
@@ -4818,7 +4818,7 @@
         <v>33</v>
       </c>
       <c r="B167" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C167">
         <v>1993</v>
@@ -4835,7 +4835,7 @@
         <v>33</v>
       </c>
       <c r="B168" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C168">
         <v>1994</v>
@@ -4849,10 +4849,10 @@
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B169" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C169">
         <v>1994</v>
@@ -4869,7 +4869,7 @@
         <v>33</v>
       </c>
       <c r="B170" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C170">
         <v>1995</v>
@@ -4883,10 +4883,10 @@
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B171" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C171">
         <v>1995</v>
@@ -4903,7 +4903,7 @@
         <v>33</v>
       </c>
       <c r="B172" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C172">
         <v>1995</v>
@@ -4917,10 +4917,10 @@
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B173" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C173">
         <v>1997</v>
@@ -4932,7 +4932,7 @@
         <v>40</v>
       </c>
       <c r="F173" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
@@ -4940,7 +4940,7 @@
         <v>33</v>
       </c>
       <c r="B174" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C174">
         <v>1998</v>
@@ -4949,15 +4949,15 @@
         <v>9999</v>
       </c>
       <c r="E174" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B175" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C175">
         <v>1998</v>
@@ -4969,12 +4969,12 @@
         <v>40</v>
       </c>
       <c r="F175" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B176" t="s">
         <v>60</v>
@@ -4989,15 +4989,15 @@
         <v>40</v>
       </c>
       <c r="F176" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B177" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C177">
         <v>2002</v>
@@ -5006,7 +5006,7 @@
         <v>9999</v>
       </c>
       <c r="E177" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -5014,7 +5014,7 @@
         <v>33</v>
       </c>
       <c r="B178" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C178">
         <v>2002</v>
@@ -5028,10 +5028,10 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B179" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C179">
         <v>2003</v>
@@ -5045,10 +5045,10 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B180" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C180">
         <v>2002</v>
@@ -5062,10 +5062,10 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B181" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C181">
         <v>2003</v>
@@ -5074,7 +5074,7 @@
         <v>9999</v>
       </c>
       <c r="E181" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
@@ -5082,7 +5082,7 @@
         <v>33</v>
       </c>
       <c r="B182" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C182">
         <v>2003</v>
@@ -5096,13 +5096,13 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>297</v>
+        <v>378</v>
       </c>
       <c r="B183" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C183">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="D183">
         <v>9999</v>
@@ -5116,7 +5116,7 @@
         <v>33</v>
       </c>
       <c r="B184" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C184">
         <v>2004</v>
@@ -5130,10 +5130,10 @@
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B185" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C185">
         <v>2005</v>
@@ -5142,7 +5142,7 @@
         <v>9999</v>
       </c>
       <c r="E185" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
@@ -5150,7 +5150,7 @@
         <v>33</v>
       </c>
       <c r="B186" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C186">
         <v>2005</v>
@@ -5167,7 +5167,7 @@
         <v>33</v>
       </c>
       <c r="B187" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C187">
         <v>2005</v>
@@ -5181,10 +5181,10 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B188" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C188">
         <v>2006</v>
@@ -5193,15 +5193,15 @@
         <v>9999</v>
       </c>
       <c r="E188" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B189" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C189">
         <v>2007</v>
@@ -5210,15 +5210,15 @@
         <v>9999</v>
       </c>
       <c r="E189" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B190" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C190">
         <v>2007</v>
@@ -5232,10 +5232,10 @@
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B191" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C191">
         <v>2008</v>
@@ -5244,7 +5244,7 @@
         <v>9999</v>
       </c>
       <c r="E191" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -5252,7 +5252,7 @@
         <v>33</v>
       </c>
       <c r="B192" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C192">
         <v>2008</v>
@@ -5261,15 +5261,15 @@
         <v>9999</v>
       </c>
       <c r="E192" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B193" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C193">
         <v>2009</v>
@@ -5278,7 +5278,7 @@
         <v>9999</v>
       </c>
       <c r="E193" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
@@ -5286,7 +5286,7 @@
         <v>33</v>
       </c>
       <c r="B194" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C194">
         <v>2009</v>
@@ -5300,10 +5300,10 @@
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B195" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C195">
         <v>2009</v>
@@ -5320,7 +5320,7 @@
         <v>33</v>
       </c>
       <c r="B196" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C196">
         <v>2010</v>
@@ -5329,15 +5329,15 @@
         <v>9999</v>
       </c>
       <c r="E196" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B197" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C197">
         <v>2012</v>
@@ -5346,15 +5346,15 @@
         <v>9999</v>
       </c>
       <c r="E197" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B198" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C198">
         <v>2012</v>
@@ -5363,15 +5363,15 @@
         <v>9999</v>
       </c>
       <c r="E198" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B199" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C199">
         <v>2013</v>
@@ -5380,15 +5380,15 @@
         <v>9999</v>
       </c>
       <c r="E199" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B200" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C200">
         <v>2014</v>
@@ -5397,7 +5397,7 @@
         <v>9999</v>
       </c>
       <c r="E200" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -5405,7 +5405,7 @@
         <v>33</v>
       </c>
       <c r="B201" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C201">
         <v>2014</v>
@@ -5419,10 +5419,10 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B202" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C202">
         <v>2015</v>
@@ -5431,15 +5431,15 @@
         <v>9999</v>
       </c>
       <c r="E202" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B203" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C203">
         <v>2015</v>
@@ -5448,15 +5448,15 @@
         <v>9999</v>
       </c>
       <c r="E203" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B204" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="C204">
         <v>2015</v>
@@ -5465,7 +5465,7 @@
         <v>9999</v>
       </c>
       <c r="E204" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
@@ -5473,7 +5473,7 @@
         <v>33</v>
       </c>
       <c r="B205" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C205">
         <v>2016</v>
@@ -5490,7 +5490,7 @@
         <v>33</v>
       </c>
       <c r="B206" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C206">
         <v>2017</v>
@@ -5504,10 +5504,10 @@
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B207" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C207">
         <v>2018</v>
@@ -5516,15 +5516,15 @@
         <v>9999</v>
       </c>
       <c r="E207" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B208" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C208">
         <v>2018</v>
@@ -5533,15 +5533,15 @@
         <v>9999</v>
       </c>
       <c r="E208" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B209" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C209">
         <v>2018</v>
@@ -5555,10 +5555,10 @@
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B210" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C210">
         <v>2019</v>
@@ -5567,15 +5567,15 @@
         <v>9999</v>
       </c>
       <c r="E210" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B211" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="C211">
         <v>2021</v>

</xml_diff>

<commit_message>
Updates based on Ken's 2nd pass review of Tom Humphrey's material.
</commit_message>
<xml_diff>
--- a/xlsx/feature_timeline.xlsx
+++ b/xlsx/feature_timeline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\historical-transportation-map\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kend/Documents/General Maps/Time Line/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77724871-E7C2-45E1-956C-63B8CA4935A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A079EF-B386-0441-BA90-71014E15E4DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="18460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="feature_timeline" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="368">
   <si>
     <t>layer_name</t>
   </si>
@@ -502,9 +502,6 @@
     <t>Worcester-CR-1994</t>
   </si>
   <si>
-    <t>SE Expressway HOV lane</t>
-  </si>
-  <si>
     <t>Ted-Williams-Tunnel-1995</t>
   </si>
   <si>
@@ -772,9 +769,6 @@
     <t>Cambridge-Concord Turnpike, made public highway</t>
   </si>
   <si>
-    <t>Route 3 completed</t>
-  </si>
-  <si>
     <t>Interstate 495 (Chelmsford–Littleton)</t>
   </si>
   <si>
@@ -904,15 +898,6 @@
     <t>Interstate 95 (Boxford–Newburyport)</t>
   </si>
   <si>
-    <t>Route 3 (I-495–Route 128)</t>
-  </si>
-  <si>
-    <t>Interstate 93 (Fort Hill–SE Expressway)</t>
-  </si>
-  <si>
-    <t>Interstate 93 (SE Expressway–Route 3–Route 24–I-95)</t>
-  </si>
-  <si>
     <t>Route 24 (Brockton–Route 128)</t>
   </si>
   <si>
@@ -1051,9 +1036,6 @@
     <t>Route 128 (Wakefield–Wellesley)</t>
   </si>
   <si>
-    <t>Route 3 B148completed</t>
-  </si>
-  <si>
     <t>Fairmount Commuter Rail line</t>
   </si>
   <si>
@@ -1088,6 +1070,60 @@
   </si>
   <si>
     <t>Orange Line (Chinatown–Dudley Square)</t>
+  </si>
+  <si>
+    <t>National Transportation Safety Board founded</t>
+  </si>
+  <si>
+    <t>US-Rt-1-North</t>
+  </si>
+  <si>
+    <t>US Route 1</t>
+  </si>
+  <si>
+    <t>I95-Boxford</t>
+  </si>
+  <si>
+    <t>I95-direct</t>
+  </si>
+  <si>
+    <t>Interstate 95 (Saugus–Canton)</t>
+  </si>
+  <si>
+    <t>I95-South</t>
+  </si>
+  <si>
+    <t>US Route 3 (I-495–Route 128)</t>
+  </si>
+  <si>
+    <t>Route-3-Boston-Norwell-1957</t>
+  </si>
+  <si>
+    <t>Route 3 (I-93-Norwell)</t>
+  </si>
+  <si>
+    <t>Route 3 (Norwell–Bourne)</t>
+  </si>
+  <si>
+    <t>Southeast Expressway HOV lane</t>
+  </si>
+  <si>
+    <t>Interstate 93 (Fort Hill–Southeast Expressway)</t>
+  </si>
+  <si>
+    <t>Interstate 93 (Southeast Expressway–Route 3–Route 24–I-95)</t>
+  </si>
+  <si>
+    <t>Red_Line-1928</t>
+  </si>
+  <si>
+    <t>Old_Colony_Fall_River_RR-1847-1863</t>
+  </si>
+  <si>
+    <t>Upper_Charles_Rail_Trail-2015</t>
+  </si>
+  <si>
+    <t>Upper Charles Rail Trail (Milford, Holliston)</t>
   </si>
 </sst>
 </file>
@@ -1928,22 +1964,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F200"/>
+  <dimension ref="A1:F204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
+      <selection activeCell="F148" sqref="F148"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="6" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelRow="6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1960,10 +1996,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1977,7 +2013,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1991,7 +2027,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2005,7 +2041,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -2019,7 +2055,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2033,7 +2069,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -2047,7 +2083,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -2061,7 +2097,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -2075,7 +2111,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -2089,7 +2125,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -2103,12 +2139,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C12">
         <v>1803</v>
@@ -2120,12 +2156,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C13">
         <v>1805</v>
@@ -2137,29 +2173,29 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C14">
         <v>1807</v>
       </c>
       <c r="D14">
-        <v>9999</v>
+        <v>1830</v>
       </c>
       <c r="E14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C15">
         <v>1808</v>
@@ -2171,12 +2207,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C16">
         <v>1808</v>
@@ -2188,29 +2224,29 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C17">
         <v>1809</v>
       </c>
       <c r="D17">
-        <v>1965</v>
+        <v>1830</v>
       </c>
       <c r="E17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C18">
         <v>1811</v>
@@ -2222,12 +2258,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C19">
         <v>1817</v>
@@ -2239,12 +2275,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C20">
         <v>1825</v>
@@ -2256,12 +2292,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C21">
         <v>1826</v>
@@ -2273,12 +2309,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C22">
         <v>1826</v>
@@ -2290,12 +2326,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C23">
         <v>1829</v>
@@ -2307,12 +2343,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C24">
         <v>1830</v>
@@ -2324,12 +2360,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="C25">
         <v>1834</v>
@@ -2341,12 +2377,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="C26">
         <v>1834</v>
@@ -2358,12 +2394,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="C27">
         <v>1835</v>
@@ -2375,12 +2411,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="C28">
         <v>1836</v>
@@ -2392,12 +2428,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C29">
         <v>1838</v>
@@ -2409,12 +2445,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="C30">
         <v>1838</v>
@@ -2426,12 +2462,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B31" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C31">
         <v>1838</v>
@@ -2443,12 +2479,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>37</v>
       </c>
       <c r="B32" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="C32">
         <v>1839</v>
@@ -2460,12 +2496,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>38</v>
       </c>
       <c r="B33" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="C33">
         <v>1840</v>
@@ -2477,12 +2513,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="C34">
         <v>1843</v>
@@ -2494,12 +2530,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C35">
         <v>1843</v>
@@ -2511,12 +2547,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B36" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="C36">
         <v>1844</v>
@@ -2528,12 +2564,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>40</v>
       </c>
       <c r="B37" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="C37">
         <v>1844</v>
@@ -2545,7 +2581,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -2562,12 +2598,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>43</v>
       </c>
       <c r="B39" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="C39">
         <v>1845</v>
@@ -2579,12 +2615,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>44</v>
       </c>
       <c r="B40" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="C40">
         <v>1845</v>
@@ -2596,12 +2632,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>25</v>
+        <v>365</v>
       </c>
       <c r="B41" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="C41">
         <v>1846</v>
@@ -2613,12 +2649,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B42" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C42">
         <v>1846</v>
@@ -2630,12 +2666,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="C43">
         <v>1847</v>
@@ -2647,12 +2683,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B44" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="C44">
         <v>1847</v>
@@ -2664,12 +2700,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B45" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C45">
         <v>1847</v>
@@ -2681,12 +2717,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B46" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C46">
         <v>1848</v>
@@ -2698,12 +2734,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="C47">
         <v>1849</v>
@@ -2715,12 +2751,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="C48">
         <v>1849</v>
@@ -2732,12 +2768,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="C49">
         <v>1850</v>
@@ -2749,9 +2785,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B50" t="s">
         <v>49</v>
@@ -2766,12 +2802,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B51" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C51">
         <v>1850</v>
@@ -2783,12 +2819,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B52" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C52">
         <v>1850</v>
@@ -2800,12 +2836,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B53" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C53">
         <v>1852</v>
@@ -2817,12 +2853,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B54" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C54">
         <v>1853</v>
@@ -2834,12 +2870,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B55" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="C55">
         <v>1853</v>
@@ -2851,12 +2887,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>25</v>
       </c>
       <c r="B56" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C56">
         <v>1856</v>
@@ -2868,12 +2904,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>50</v>
       </c>
       <c r="B57" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C57">
         <v>1857</v>
@@ -2885,12 +2921,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>51</v>
       </c>
       <c r="B58" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="C58">
         <v>1861</v>
@@ -2902,12 +2938,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>52</v>
       </c>
       <c r="B59" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C59">
         <v>1861</v>
@@ -2919,12 +2955,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B60" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C60">
         <v>1867</v>
@@ -2936,7 +2972,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>53</v>
       </c>
@@ -2953,12 +2989,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B62" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C62">
         <v>1868</v>
@@ -2970,12 +3006,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B63" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C63">
         <v>1846</v>
@@ -2987,12 +3023,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B64" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C64">
         <v>1871</v>
@@ -3004,12 +3040,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B65" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C65">
         <v>1874</v>
@@ -3021,12 +3057,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>55</v>
       </c>
       <c r="B66" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C66">
         <v>1875</v>
@@ -3038,12 +3074,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>56</v>
       </c>
       <c r="B67" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="C67">
         <v>1888</v>
@@ -3055,7 +3091,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>57</v>
       </c>
@@ -3072,7 +3108,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>59</v>
       </c>
@@ -3089,7 +3125,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>25</v>
       </c>
@@ -3106,7 +3142,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>25</v>
       </c>
@@ -3123,7 +3159,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>64</v>
       </c>
@@ -3140,7 +3176,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>66</v>
       </c>
@@ -3157,7 +3193,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>25</v>
       </c>
@@ -3174,12 +3210,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>69</v>
       </c>
       <c r="B75" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="C75">
         <v>1901</v>
@@ -3191,7 +3227,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>70</v>
       </c>
@@ -3208,12 +3244,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>72</v>
       </c>
       <c r="B77" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C77">
         <v>1901</v>
@@ -3225,7 +3261,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>25</v>
       </c>
@@ -3242,7 +3278,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>74</v>
       </c>
@@ -3259,12 +3295,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>76</v>
       </c>
       <c r="B80" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="C80">
         <v>1907</v>
@@ -3276,12 +3312,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B81" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C81">
         <v>1909</v>
@@ -3293,12 +3329,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>77</v>
       </c>
       <c r="B82" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C82">
         <v>1912</v>
@@ -3310,7 +3346,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>78</v>
       </c>
@@ -3327,7 +3363,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>25</v>
       </c>
@@ -3344,12 +3380,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>81</v>
       </c>
       <c r="B85" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C85">
         <v>1914</v>
@@ -3361,12 +3397,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>82</v>
       </c>
       <c r="B86" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="C86">
         <v>1915</v>
@@ -3378,12 +3414,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>83</v>
       </c>
       <c r="B87" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C87">
         <v>1916</v>
@@ -3395,12 +3431,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B88" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="C88">
         <v>1917</v>
@@ -3412,12 +3448,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>84</v>
       </c>
       <c r="B89" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C89">
         <v>1918</v>
@@ -3429,7 +3465,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>25</v>
       </c>
@@ -3446,12 +3482,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>86</v>
       </c>
       <c r="B91" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C91">
         <v>1919</v>
@@ -3463,7 +3499,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>25</v>
       </c>
@@ -3480,7 +3516,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>88</v>
       </c>
@@ -3497,32 +3533,32 @@
         <v>90</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
+        <v>351</v>
+      </c>
+      <c r="B94" t="s">
+        <v>352</v>
+      </c>
+      <c r="C94">
+        <v>1926</v>
+      </c>
+      <c r="D94">
+        <v>9999</v>
+      </c>
+      <c r="E94" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
         <v>91</v>
       </c>
-      <c r="B94" t="s">
-        <v>339</v>
-      </c>
-      <c r="C94">
+      <c r="B95" t="s">
+        <v>334</v>
+      </c>
+      <c r="C95">
         <v>1927</v>
-      </c>
-      <c r="D94">
-        <v>9999</v>
-      </c>
-      <c r="E94" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>76</v>
-      </c>
-      <c r="B95" t="s">
-        <v>340</v>
-      </c>
-      <c r="C95">
-        <v>1928</v>
       </c>
       <c r="D95">
         <v>9999</v>
@@ -3531,15 +3567,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>92</v>
+        <v>364</v>
       </c>
       <c r="B96" t="s">
-        <v>93</v>
+        <v>335</v>
       </c>
       <c r="C96">
-        <v>1929</v>
+        <v>1928</v>
       </c>
       <c r="D96">
         <v>9999</v>
@@ -3548,80 +3584,80 @@
         <v>27</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>25</v>
+        <v>92</v>
       </c>
       <c r="B97" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C97">
-        <v>1930</v>
+        <v>1929</v>
       </c>
       <c r="D97">
-        <v>1983</v>
+        <v>9999</v>
       </c>
       <c r="E97" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
+        <v>25</v>
+      </c>
+      <c r="B98" t="s">
+        <v>94</v>
+      </c>
+      <c r="C98">
+        <v>1930</v>
+      </c>
+      <c r="D98">
+        <v>1983</v>
+      </c>
+      <c r="E98" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
         <v>95</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B99" t="s">
         <v>96</v>
       </c>
-      <c r="C98">
+      <c r="C99">
         <v>1934</v>
       </c>
-      <c r="D98">
-        <v>9999</v>
-      </c>
-      <c r="E98" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+      <c r="D99">
+        <v>9999</v>
+      </c>
+      <c r="E99" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
         <v>25</v>
       </c>
-      <c r="B99" t="s">
-        <v>289</v>
-      </c>
-      <c r="C99">
+      <c r="B100" t="s">
+        <v>287</v>
+      </c>
+      <c r="C100">
         <v>1936</v>
       </c>
-      <c r="D99">
+      <c r="D100">
         <v>1963</v>
       </c>
-      <c r="E99" t="s">
+      <c r="E100" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
         <v>97</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B101" t="s">
         <v>98</v>
-      </c>
-      <c r="C100">
-        <v>1941</v>
-      </c>
-      <c r="D100">
-        <v>9999</v>
-      </c>
-      <c r="E100" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>99</v>
-      </c>
-      <c r="B101" t="s">
-        <v>341</v>
       </c>
       <c r="C101">
         <v>1941</v>
@@ -3630,168 +3666,168 @@
         <v>9999</v>
       </c>
       <c r="E101" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B102" t="s">
-        <v>232</v>
+        <v>336</v>
       </c>
       <c r="C102">
         <v>1941</v>
       </c>
       <c r="D102">
-        <v>1985</v>
+        <v>9999</v>
       </c>
       <c r="E102" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="B103" t="s">
-        <v>101</v>
+        <v>231</v>
       </c>
       <c r="C103">
-        <v>1943</v>
+        <v>1941</v>
       </c>
       <c r="D103">
-        <v>9999</v>
+        <v>1985</v>
       </c>
       <c r="E103" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>25</v>
       </c>
       <c r="B104" t="s">
-        <v>211</v>
+        <v>101</v>
       </c>
       <c r="C104">
+        <v>1943</v>
+      </c>
+      <c r="D104">
+        <v>9999</v>
+      </c>
+      <c r="E104" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>25</v>
+      </c>
+      <c r="B105" t="s">
+        <v>210</v>
+      </c>
+      <c r="C105">
         <v>1947</v>
       </c>
-      <c r="D104">
+      <c r="D105">
         <v>1964</v>
       </c>
-      <c r="E104" t="s">
+      <c r="E105" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
         <v>102</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B106" t="s">
         <v>103</v>
       </c>
-      <c r="C105">
+      <c r="C106">
         <v>1950</v>
       </c>
-      <c r="D105">
-        <v>9999</v>
-      </c>
-      <c r="E105" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+      <c r="D106">
+        <v>9999</v>
+      </c>
+      <c r="E106" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
         <v>104</v>
       </c>
-      <c r="B106" t="s">
-        <v>342</v>
-      </c>
-      <c r="C106">
+      <c r="B107" t="s">
+        <v>337</v>
+      </c>
+      <c r="C107">
         <v>1951</v>
       </c>
-      <c r="D106">
-        <v>9999</v>
-      </c>
-      <c r="E106" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+      <c r="D107">
+        <v>9999</v>
+      </c>
+      <c r="E107" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
         <v>105</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B108" t="s">
         <v>106</v>
-      </c>
-      <c r="C107">
-        <v>1952</v>
-      </c>
-      <c r="D107">
-        <v>9999</v>
-      </c>
-      <c r="E107" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>25</v>
-      </c>
-      <c r="B108" t="s">
-        <v>107</v>
       </c>
       <c r="C108">
         <v>1952</v>
       </c>
       <c r="D108">
-        <v>2009</v>
+        <v>9999</v>
       </c>
       <c r="E108" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>108</v>
+        <v>25</v>
       </c>
       <c r="B109" t="s">
-        <v>290</v>
+        <v>107</v>
       </c>
       <c r="C109">
         <v>1952</v>
       </c>
       <c r="D109">
-        <v>9999</v>
+        <v>2009</v>
       </c>
       <c r="E109" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>108</v>
+      </c>
+      <c r="B110" t="s">
+        <v>288</v>
+      </c>
+      <c r="C110">
+        <v>1952</v>
+      </c>
+      <c r="D110">
+        <v>9999</v>
+      </c>
+      <c r="E110" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
         <v>109</v>
       </c>
-      <c r="B110" t="s">
-        <v>291</v>
-      </c>
-      <c r="C110">
-        <v>1954</v>
-      </c>
-      <c r="D110">
-        <v>9999</v>
-      </c>
-      <c r="E110" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>111</v>
-      </c>
       <c r="B111" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C111">
         <v>1954</v>
@@ -3800,15 +3836,15 @@
         <v>9999</v>
       </c>
       <c r="E111" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C112">
         <v>1954</v>
@@ -3817,168 +3853,165 @@
         <v>9999</v>
       </c>
       <c r="E112" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
+        <v>353</v>
+      </c>
+      <c r="B113" t="s">
+        <v>291</v>
+      </c>
+      <c r="C113">
+        <v>1954</v>
+      </c>
+      <c r="D113">
+        <v>9999</v>
+      </c>
+      <c r="E113" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>112</v>
+      </c>
+      <c r="B114" t="s">
+        <v>355</v>
+      </c>
+      <c r="C114">
+        <v>1954</v>
+      </c>
+      <c r="D114">
+        <v>9999</v>
+      </c>
+      <c r="E114" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
         <v>110</v>
       </c>
-      <c r="B113" t="s">
-        <v>294</v>
-      </c>
-      <c r="C113">
+      <c r="B115" t="s">
+        <v>357</v>
+      </c>
+      <c r="C115">
         <v>1955</v>
       </c>
-      <c r="D113">
-        <v>9999</v>
-      </c>
-      <c r="E113" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+      <c r="D115">
+        <v>9999</v>
+      </c>
+      <c r="E115" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
         <v>25</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B116" t="s">
         <v>113</v>
       </c>
-      <c r="C114">
+      <c r="C116">
         <v>1956</v>
       </c>
-      <c r="D114">
-        <v>9999</v>
-      </c>
-      <c r="E114" t="s">
+      <c r="D116">
+        <v>9999</v>
+      </c>
+      <c r="E116" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
         <v>25</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B117" t="s">
         <v>114</v>
       </c>
-      <c r="C115">
+      <c r="C117">
         <v>1957</v>
       </c>
-      <c r="D115">
+      <c r="D117">
         <v>2016</v>
       </c>
-      <c r="E115" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+      <c r="E117" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
         <v>115</v>
       </c>
-      <c r="B116" t="s">
-        <v>254</v>
-      </c>
-      <c r="C116">
+      <c r="B118" t="s">
+        <v>252</v>
+      </c>
+      <c r="C118">
         <v>1957</v>
       </c>
-      <c r="D116">
-        <v>9999</v>
-      </c>
-      <c r="E116" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+      <c r="D118">
+        <v>9999</v>
+      </c>
+      <c r="E118" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>358</v>
+      </c>
+      <c r="B119" t="s">
+        <v>359</v>
+      </c>
+      <c r="C119">
+        <v>1957</v>
+      </c>
+      <c r="D119">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
         <v>116</v>
       </c>
-      <c r="B117" t="s">
-        <v>295</v>
-      </c>
-      <c r="C117">
+      <c r="B120" t="s">
+        <v>362</v>
+      </c>
+      <c r="C120">
         <v>1958</v>
       </c>
-      <c r="D117">
-        <v>9999</v>
-      </c>
-      <c r="E117" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>208</v>
-      </c>
-      <c r="B118" t="s">
-        <v>296</v>
-      </c>
-      <c r="C118">
+      <c r="D120">
+        <v>9999</v>
+      </c>
+      <c r="E120" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>207</v>
+      </c>
+      <c r="B121" t="s">
+        <v>363</v>
+      </c>
+      <c r="C121">
         <v>1958</v>
       </c>
-      <c r="D118">
-        <v>9999</v>
-      </c>
-      <c r="E118" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+      <c r="D121">
+        <v>9999</v>
+      </c>
+      <c r="E121" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
         <v>117</v>
       </c>
-      <c r="B119" t="s">
-        <v>297</v>
-      </c>
-      <c r="C119">
-        <v>1959</v>
-      </c>
-      <c r="D119">
-        <v>9999</v>
-      </c>
-      <c r="E119" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>25</v>
-      </c>
-      <c r="B120" t="s">
-        <v>118</v>
-      </c>
-      <c r="C120">
-        <v>1959</v>
-      </c>
-      <c r="D120">
-        <v>2004</v>
-      </c>
-      <c r="E120" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>25</v>
-      </c>
-      <c r="B121" t="s">
-        <v>119</v>
-      </c>
-      <c r="C121">
-        <v>1959</v>
-      </c>
-      <c r="D121">
-        <v>9999</v>
-      </c>
-      <c r="E121" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>120</v>
-      </c>
       <c r="B122" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="C122">
         <v>1959</v>
@@ -3987,66 +4020,66 @@
         <v>9999</v>
       </c>
       <c r="E122" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>25</v>
+      </c>
+      <c r="B123" t="s">
+        <v>118</v>
+      </c>
+      <c r="C123">
+        <v>1959</v>
+      </c>
+      <c r="D123">
+        <v>2004</v>
+      </c>
+      <c r="E123" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>25</v>
+      </c>
+      <c r="B124" t="s">
+        <v>119</v>
+      </c>
+      <c r="C124">
+        <v>1959</v>
+      </c>
+      <c r="D124">
+        <v>9999</v>
+      </c>
+      <c r="E124" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>120</v>
+      </c>
+      <c r="B125" t="s">
+        <v>293</v>
+      </c>
+      <c r="C125">
+        <v>1959</v>
+      </c>
+      <c r="D125">
+        <v>9999</v>
+      </c>
+      <c r="E125" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>121</v>
-      </c>
-      <c r="B123" t="s">
-        <v>250</v>
-      </c>
-      <c r="C123">
-        <v>1963</v>
-      </c>
-      <c r="D123">
-        <v>9999</v>
-      </c>
-      <c r="E123" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
         <v>122</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B126" t="s">
         <v>123</v>
-      </c>
-      <c r="C124">
-        <v>1962</v>
-      </c>
-      <c r="D124">
-        <v>9999</v>
-      </c>
-      <c r="E124" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>124</v>
-      </c>
-      <c r="B125" t="s">
-        <v>251</v>
-      </c>
-      <c r="C125">
-        <v>1961</v>
-      </c>
-      <c r="D125">
-        <v>9999</v>
-      </c>
-      <c r="E125" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>110</v>
-      </c>
-      <c r="B126" t="s">
-        <v>126</v>
       </c>
       <c r="C126">
         <v>1962</v>
@@ -4058,60 +4091,63 @@
         <v>17</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>252</v>
+        <v>124</v>
       </c>
       <c r="B127" t="s">
-        <v>299</v>
+        <v>249</v>
       </c>
       <c r="C127">
+        <v>1961</v>
+      </c>
+      <c r="D127">
+        <v>9999</v>
+      </c>
+      <c r="E127" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>110</v>
+      </c>
+      <c r="B128" t="s">
+        <v>126</v>
+      </c>
+      <c r="C128">
         <v>1962</v>
       </c>
-      <c r="D127">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
+      <c r="D128">
+        <v>9999</v>
+      </c>
+      <c r="E128" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>250</v>
+      </c>
+      <c r="B129" t="s">
+        <v>294</v>
+      </c>
+      <c r="C129">
+        <v>1962</v>
+      </c>
+      <c r="D129">
+        <v>9999</v>
+      </c>
+      <c r="E129" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
         <v>127</v>
       </c>
-      <c r="B128" t="s">
-        <v>300</v>
-      </c>
-      <c r="C128">
-        <v>1964</v>
-      </c>
-      <c r="D128">
-        <v>9999</v>
-      </c>
-      <c r="E128" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>121</v>
-      </c>
-      <c r="B129" t="s">
-        <v>343</v>
-      </c>
-      <c r="C129">
-        <v>1963</v>
-      </c>
-      <c r="D129">
-        <v>9999</v>
-      </c>
-      <c r="E129" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>128</v>
-      </c>
       <c r="B130" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="C130">
         <v>1964</v>
@@ -4123,15 +4159,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B131" t="s">
-        <v>302</v>
+        <v>360</v>
       </c>
       <c r="C131">
-        <v>1960</v>
+        <v>1961</v>
       </c>
       <c r="D131">
         <v>9999</v>
@@ -4140,12 +4176,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>25</v>
+        <v>128</v>
       </c>
       <c r="B132" t="s">
-        <v>130</v>
+        <v>296</v>
       </c>
       <c r="C132">
         <v>1964</v>
@@ -4154,49 +4190,49 @@
         <v>9999</v>
       </c>
       <c r="E132" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
+        <v>129</v>
+      </c>
+      <c r="B133" t="s">
+        <v>297</v>
+      </c>
+      <c r="C133">
+        <v>1960</v>
+      </c>
+      <c r="D133">
+        <v>9999</v>
+      </c>
+      <c r="E133" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>25</v>
+      </c>
+      <c r="B134" t="s">
+        <v>130</v>
+      </c>
+      <c r="C134">
+        <v>1964</v>
+      </c>
+      <c r="D134">
+        <v>9999</v>
+      </c>
+      <c r="E134" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
         <v>131</v>
       </c>
-      <c r="B133" t="s">
-        <v>303</v>
-      </c>
-      <c r="C133">
-        <v>1965</v>
-      </c>
-      <c r="D133">
-        <v>9999</v>
-      </c>
-      <c r="E133" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>112</v>
-      </c>
-      <c r="B134" t="s">
-        <v>304</v>
-      </c>
-      <c r="C134">
-        <v>1965</v>
-      </c>
-      <c r="D134">
-        <v>9999</v>
-      </c>
-      <c r="E134" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>132</v>
-      </c>
       <c r="B135" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="C135">
         <v>1965</v>
@@ -4208,199 +4244,199 @@
         <v>17</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>253</v>
+        <v>356</v>
       </c>
       <c r="B136" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="C136">
+        <v>1965</v>
+      </c>
+      <c r="D136">
+        <v>9999</v>
+      </c>
+      <c r="E136" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>132</v>
+      </c>
+      <c r="B137" t="s">
+        <v>300</v>
+      </c>
+      <c r="C137">
+        <v>1965</v>
+      </c>
+      <c r="D137">
+        <v>9999</v>
+      </c>
+      <c r="E137" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>25</v>
+      </c>
+      <c r="B138" t="s">
+        <v>350</v>
+      </c>
+      <c r="C138">
+        <v>1967</v>
+      </c>
+      <c r="D138">
+        <v>9999</v>
+      </c>
+      <c r="E138" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>251</v>
+      </c>
+      <c r="B139" t="s">
+        <v>301</v>
+      </c>
+      <c r="C139">
         <v>1968</v>
       </c>
-      <c r="D136">
-        <v>9999</v>
-      </c>
-      <c r="E136" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
+      <c r="D139">
+        <v>9999</v>
+      </c>
+      <c r="E139" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
         <v>133</v>
       </c>
-      <c r="B137" t="s">
-        <v>307</v>
-      </c>
-      <c r="C137">
+      <c r="B140" t="s">
+        <v>302</v>
+      </c>
+      <c r="C140">
         <v>1969</v>
       </c>
-      <c r="D137">
-        <v>9999</v>
-      </c>
-      <c r="E137" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
+      <c r="D140">
+        <v>9999</v>
+      </c>
+      <c r="E140" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
         <v>134</v>
       </c>
-      <c r="B138" t="s">
-        <v>308</v>
-      </c>
-      <c r="C138">
+      <c r="B141" t="s">
+        <v>303</v>
+      </c>
+      <c r="C141">
         <v>1966</v>
       </c>
-      <c r="D138">
-        <v>9999</v>
-      </c>
-      <c r="E138" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
+      <c r="D141">
+        <v>9999</v>
+      </c>
+      <c r="E141" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
         <v>135</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B142" t="s">
         <v>136</v>
       </c>
-      <c r="C139">
+      <c r="C142">
         <v>1970</v>
       </c>
-      <c r="D139">
-        <v>9999</v>
-      </c>
-      <c r="E139" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
+      <c r="D142">
+        <v>9999</v>
+      </c>
+      <c r="E142" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
         <v>137</v>
       </c>
-      <c r="B140" t="s">
-        <v>309</v>
-      </c>
-      <c r="C140">
+      <c r="B143" t="s">
+        <v>304</v>
+      </c>
+      <c r="C143">
         <v>1971</v>
       </c>
-      <c r="D140">
-        <v>9999</v>
-      </c>
-      <c r="E140" t="s">
+      <c r="D143">
+        <v>9999</v>
+      </c>
+      <c r="E143" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
         <v>138</v>
       </c>
-      <c r="B141" t="s">
-        <v>310</v>
-      </c>
-      <c r="C141">
+      <c r="B144" t="s">
+        <v>305</v>
+      </c>
+      <c r="C144">
         <v>1973</v>
       </c>
-      <c r="D141">
-        <v>9999</v>
-      </c>
-      <c r="E141" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>25</v>
-      </c>
-      <c r="B142" t="s">
-        <v>238</v>
-      </c>
-      <c r="C142">
-        <v>1973</v>
-      </c>
-      <c r="D142">
-        <v>9999</v>
-      </c>
-      <c r="E142" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>25</v>
-      </c>
-      <c r="B143" t="s">
-        <v>139</v>
-      </c>
-      <c r="C143">
-        <v>1974</v>
-      </c>
-      <c r="D143">
-        <v>9999</v>
-      </c>
-      <c r="E143" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>140</v>
-      </c>
-      <c r="B144" t="s">
-        <v>141</v>
-      </c>
-      <c r="C144">
-        <v>1975</v>
-      </c>
       <c r="D144">
         <v>9999</v>
       </c>
       <c r="E144" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>25</v>
       </c>
       <c r="B145" t="s">
-        <v>143</v>
+        <v>237</v>
       </c>
       <c r="C145">
-        <v>1975</v>
+        <v>1973</v>
       </c>
       <c r="D145">
         <v>9999</v>
       </c>
       <c r="E145" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>125</v>
+        <v>25</v>
       </c>
       <c r="B146" t="s">
-        <v>311</v>
+        <v>139</v>
       </c>
       <c r="C146">
-        <v>1975</v>
+        <v>1974</v>
       </c>
       <c r="D146">
         <v>9999</v>
       </c>
       <c r="E146" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B147" t="s">
-        <v>312</v>
+        <v>141</v>
       </c>
       <c r="C147">
         <v>1975</v>
@@ -4409,52 +4445,52 @@
         <v>9999</v>
       </c>
       <c r="E147" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>145</v>
+        <v>25</v>
       </c>
       <c r="B148" t="s">
-        <v>344</v>
+        <v>143</v>
       </c>
       <c r="C148">
-        <v>1979</v>
+        <v>1975</v>
       </c>
       <c r="D148">
         <v>9999</v>
       </c>
       <c r="E148" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>25</v>
+        <v>125</v>
       </c>
       <c r="B149" t="s">
-        <v>146</v>
+        <v>306</v>
       </c>
       <c r="C149">
-        <v>1979</v>
+        <v>1975</v>
       </c>
       <c r="D149">
-        <v>1983</v>
+        <v>9999</v>
       </c>
       <c r="E149" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B150" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C150">
-        <v>1980</v>
+        <v>1975</v>
       </c>
       <c r="D150">
         <v>9999</v>
@@ -4463,66 +4499,69 @@
         <v>27</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B151" t="s">
-        <v>314</v>
+        <v>338</v>
       </c>
       <c r="C151">
-        <v>1984</v>
+        <v>1979</v>
       </c>
       <c r="D151">
         <v>9999</v>
       </c>
       <c r="E151" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="F151" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>149</v>
+        <v>25</v>
       </c>
       <c r="B152" t="s">
-        <v>315</v>
+        <v>146</v>
       </c>
       <c r="C152">
-        <v>1985</v>
+        <v>1979</v>
       </c>
       <c r="D152">
-        <v>9999</v>
+        <v>1983</v>
       </c>
       <c r="E152" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B153" t="s">
-        <v>151</v>
+        <v>308</v>
       </c>
       <c r="C153">
-        <v>1987</v>
+        <v>1980</v>
       </c>
       <c r="D153">
         <v>9999</v>
       </c>
       <c r="E153" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B154" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="C154">
-        <v>1987</v>
+        <v>1984</v>
       </c>
       <c r="D154">
         <v>9999</v>
@@ -4531,29 +4570,32 @@
         <v>27</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>25</v>
+        <v>149</v>
       </c>
       <c r="B155" t="s">
-        <v>255</v>
+        <v>310</v>
       </c>
       <c r="C155">
+        <v>1985</v>
+      </c>
+      <c r="D155">
+        <v>9999</v>
+      </c>
+      <c r="E155" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>150</v>
+      </c>
+      <c r="B156" t="s">
+        <v>151</v>
+      </c>
+      <c r="C156">
         <v>1987</v>
-      </c>
-      <c r="D155">
-        <v>9999</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>153</v>
-      </c>
-      <c r="B156" t="s">
-        <v>154</v>
-      </c>
-      <c r="C156">
-        <v>1992</v>
       </c>
       <c r="D156">
         <v>9999</v>
@@ -4562,191 +4604,185 @@
         <v>142</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
+        <v>152</v>
+      </c>
+      <c r="B157" t="s">
+        <v>311</v>
+      </c>
+      <c r="C157">
+        <v>1987</v>
+      </c>
+      <c r="D157">
+        <v>9999</v>
+      </c>
+      <c r="E157" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>354</v>
+      </c>
+      <c r="B158" t="s">
+        <v>253</v>
+      </c>
+      <c r="C158">
+        <v>1987</v>
+      </c>
+      <c r="D158">
+        <v>9999</v>
+      </c>
+      <c r="E158" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>153</v>
+      </c>
+      <c r="B159" t="s">
+        <v>154</v>
+      </c>
+      <c r="C159">
+        <v>1992</v>
+      </c>
+      <c r="D159">
+        <v>9999</v>
+      </c>
+      <c r="E159" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
         <v>155</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B160" t="s">
         <v>156</v>
       </c>
-      <c r="C157">
+      <c r="C160">
         <v>1992</v>
       </c>
-      <c r="D157">
-        <v>9999</v>
-      </c>
-      <c r="E157" t="s">
+      <c r="D160">
+        <v>9999</v>
+      </c>
+      <c r="E160" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>25</v>
-      </c>
-      <c r="B158" t="s">
-        <v>157</v>
-      </c>
-      <c r="C158">
-        <v>1993</v>
-      </c>
-      <c r="D158">
-        <v>9999</v>
-      </c>
-      <c r="E158" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>25</v>
-      </c>
-      <c r="B159" t="s">
-        <v>158</v>
-      </c>
-      <c r="C159">
-        <v>1994</v>
-      </c>
-      <c r="D159">
-        <v>9999</v>
-      </c>
-      <c r="E159" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>159</v>
-      </c>
-      <c r="B160" t="s">
-        <v>345</v>
-      </c>
-      <c r="C160">
-        <v>1994</v>
-      </c>
-      <c r="D160">
-        <v>9999</v>
-      </c>
-      <c r="E160" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>25</v>
       </c>
       <c r="B161" t="s">
+        <v>157</v>
+      </c>
+      <c r="C161">
+        <v>1993</v>
+      </c>
+      <c r="D161">
+        <v>9999</v>
+      </c>
+      <c r="E161" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>25</v>
+      </c>
+      <c r="B162" t="s">
+        <v>158</v>
+      </c>
+      <c r="C162">
+        <v>1994</v>
+      </c>
+      <c r="D162">
+        <v>9999</v>
+      </c>
+      <c r="E162" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>159</v>
+      </c>
+      <c r="B163" t="s">
+        <v>339</v>
+      </c>
+      <c r="C163">
+        <v>1994</v>
+      </c>
+      <c r="D163">
+        <v>9999</v>
+      </c>
+      <c r="E163" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>25</v>
+      </c>
+      <c r="B164" t="s">
+        <v>361</v>
+      </c>
+      <c r="C164">
+        <v>1995</v>
+      </c>
+      <c r="D164">
+        <v>9999</v>
+      </c>
+      <c r="E164" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" ht="15" customHeight="1" outlineLevel="6" collapsed="1" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
         <v>160</v>
       </c>
-      <c r="C161">
+      <c r="B165" t="s">
+        <v>161</v>
+      </c>
+      <c r="C165">
         <v>1995</v>
       </c>
-      <c r="D161">
-        <v>9999</v>
-      </c>
-      <c r="E161" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" ht="15" customHeight="1" outlineLevel="6" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>161</v>
-      </c>
-      <c r="B162" t="s">
+      <c r="D165">
+        <v>9999</v>
+      </c>
+      <c r="E165" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>25</v>
+      </c>
+      <c r="B166" t="s">
         <v>162</v>
       </c>
-      <c r="C162">
+      <c r="C166">
         <v>1995</v>
       </c>
-      <c r="D162">
-        <v>9999</v>
-      </c>
-      <c r="E162" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>25</v>
-      </c>
-      <c r="B163" t="s">
+      <c r="D166">
+        <v>9999</v>
+      </c>
+      <c r="E166" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
         <v>163</v>
       </c>
-      <c r="C163">
-        <v>1995</v>
-      </c>
-      <c r="D163">
-        <v>9999</v>
-      </c>
-      <c r="E163" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
-        <v>164</v>
-      </c>
-      <c r="B164" t="s">
-        <v>346</v>
-      </c>
-      <c r="C164">
+      <c r="B167" t="s">
+        <v>340</v>
+      </c>
+      <c r="C167">
         <v>1997</v>
-      </c>
-      <c r="D164">
-        <v>9999</v>
-      </c>
-      <c r="E164" t="s">
-        <v>28</v>
-      </c>
-      <c r="F164" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
-        <v>25</v>
-      </c>
-      <c r="B165" t="s">
-        <v>165</v>
-      </c>
-      <c r="C165">
-        <v>1998</v>
-      </c>
-      <c r="D165">
-        <v>9999</v>
-      </c>
-      <c r="E165" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>166</v>
-      </c>
-      <c r="B166" t="s">
-        <v>347</v>
-      </c>
-      <c r="C166">
-        <v>1998</v>
-      </c>
-      <c r="D166">
-        <v>9999</v>
-      </c>
-      <c r="E166" t="s">
-        <v>28</v>
-      </c>
-      <c r="F166" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
-        <v>167</v>
-      </c>
-      <c r="B167" t="s">
-        <v>348</v>
-      </c>
-      <c r="C167">
-        <v>1998</v>
       </c>
       <c r="D167">
         <v>9999</v>
@@ -4755,18 +4791,18 @@
         <v>28</v>
       </c>
       <c r="F167" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>168</v>
+        <v>25</v>
       </c>
       <c r="B168" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C168">
-        <v>2002</v>
+        <v>1998</v>
       </c>
       <c r="D168">
         <v>9999</v>
@@ -4775,46 +4811,52 @@
         <v>142</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>25</v>
+        <v>165</v>
       </c>
       <c r="B169" t="s">
-        <v>170</v>
+        <v>341</v>
       </c>
       <c r="C169">
-        <v>2002</v>
+        <v>1998</v>
       </c>
       <c r="D169">
         <v>9999</v>
       </c>
       <c r="E169" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="F169" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>228</v>
+        <v>166</v>
       </c>
       <c r="B170" t="s">
-        <v>229</v>
+        <v>342</v>
       </c>
       <c r="C170">
-        <v>2003</v>
+        <v>1998</v>
       </c>
       <c r="D170">
         <v>9999</v>
       </c>
       <c r="E170" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="F170" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B171" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C171">
         <v>2002</v>
@@ -4823,32 +4865,32 @@
         <v>9999</v>
       </c>
       <c r="E171" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>173</v>
+        <v>25</v>
       </c>
       <c r="B172" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C172">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="D172">
         <v>9999</v>
       </c>
       <c r="E172" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>25</v>
+        <v>227</v>
       </c>
       <c r="B173" t="s">
-        <v>175</v>
+        <v>228</v>
       </c>
       <c r="C173">
         <v>2003</v>
@@ -4860,15 +4902,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>231</v>
+        <v>170</v>
       </c>
       <c r="B174" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C174">
-        <v>2004</v>
+        <v>2002</v>
       </c>
       <c r="D174">
         <v>9999</v>
@@ -4877,83 +4919,83 @@
         <v>27</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
+        <v>172</v>
+      </c>
+      <c r="B175" t="s">
+        <v>173</v>
+      </c>
+      <c r="C175">
+        <v>2003</v>
+      </c>
+      <c r="D175">
+        <v>9999</v>
+      </c>
+      <c r="E175" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
         <v>25</v>
       </c>
-      <c r="B175" t="s">
-        <v>177</v>
-      </c>
-      <c r="C175">
+      <c r="B176" t="s">
+        <v>174</v>
+      </c>
+      <c r="C176">
+        <v>2003</v>
+      </c>
+      <c r="D176">
+        <v>9999</v>
+      </c>
+      <c r="E176" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>230</v>
+      </c>
+      <c r="B177" t="s">
+        <v>175</v>
+      </c>
+      <c r="C177">
         <v>2004</v>
       </c>
-      <c r="D175">
-        <v>2009</v>
-      </c>
-      <c r="E175" t="s">
+      <c r="D177">
+        <v>9999</v>
+      </c>
+      <c r="E177" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
-        <v>178</v>
-      </c>
-      <c r="B176" t="s">
-        <v>317</v>
-      </c>
-      <c r="C176">
-        <v>2005</v>
-      </c>
-      <c r="D176">
-        <v>9999</v>
-      </c>
-      <c r="E176" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
-        <v>25</v>
-      </c>
-      <c r="B177" t="s">
-        <v>179</v>
-      </c>
-      <c r="C177">
-        <v>2005</v>
-      </c>
-      <c r="D177">
-        <v>9999</v>
-      </c>
-      <c r="E177" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>25</v>
       </c>
       <c r="B178" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C178">
+        <v>2004</v>
+      </c>
+      <c r="D178">
+        <v>2009</v>
+      </c>
+      <c r="E178" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>177</v>
+      </c>
+      <c r="B179" t="s">
+        <v>312</v>
+      </c>
+      <c r="C179">
         <v>2005</v>
-      </c>
-      <c r="D178">
-        <v>9999</v>
-      </c>
-      <c r="E178" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>257</v>
-      </c>
-      <c r="B179" t="s">
-        <v>318</v>
-      </c>
-      <c r="C179">
-        <v>2006</v>
       </c>
       <c r="D179">
         <v>9999</v>
@@ -4962,32 +5004,32 @@
         <v>142</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>181</v>
+        <v>25</v>
       </c>
       <c r="B180" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C180">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="D180">
         <v>9999</v>
       </c>
       <c r="E180" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>183</v>
+        <v>25</v>
       </c>
       <c r="B181" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C181">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="D181">
         <v>9999</v>
@@ -4996,15 +5038,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>185</v>
+        <v>255</v>
       </c>
       <c r="B182" t="s">
-        <v>186</v>
+        <v>313</v>
       </c>
       <c r="C182">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="D182">
         <v>9999</v>
@@ -5013,15 +5055,15 @@
         <v>142</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>25</v>
+        <v>180</v>
       </c>
       <c r="B183" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="C183">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="D183">
         <v>9999</v>
@@ -5030,66 +5072,66 @@
         <v>142</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
+        <v>182</v>
+      </c>
+      <c r="B184" t="s">
+        <v>183</v>
+      </c>
+      <c r="C184">
+        <v>2007</v>
+      </c>
+      <c r="D184">
+        <v>9999</v>
+      </c>
+      <c r="E184" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>184</v>
+      </c>
+      <c r="B185" t="s">
+        <v>185</v>
+      </c>
+      <c r="C185">
+        <v>2008</v>
+      </c>
+      <c r="D185">
+        <v>9999</v>
+      </c>
+      <c r="E185" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>25</v>
+      </c>
+      <c r="B186" t="s">
+        <v>186</v>
+      </c>
+      <c r="C186">
+        <v>2008</v>
+      </c>
+      <c r="D186">
+        <v>9999</v>
+      </c>
+      <c r="E186" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>187</v>
+      </c>
+      <c r="B187" t="s">
         <v>188</v>
       </c>
-      <c r="B184" t="s">
-        <v>189</v>
-      </c>
-      <c r="C184">
+      <c r="C187">
         <v>2009</v>
-      </c>
-      <c r="D184">
-        <v>9999</v>
-      </c>
-      <c r="E184" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
-        <v>25</v>
-      </c>
-      <c r="B185" t="s">
-        <v>190</v>
-      </c>
-      <c r="C185">
-        <v>2009</v>
-      </c>
-      <c r="D185">
-        <v>9999</v>
-      </c>
-      <c r="E185" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
-        <v>191</v>
-      </c>
-      <c r="B186" t="s">
-        <v>192</v>
-      </c>
-      <c r="C186">
-        <v>2009</v>
-      </c>
-      <c r="D186">
-        <v>9999</v>
-      </c>
-      <c r="E186" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
-        <v>25</v>
-      </c>
-      <c r="B187" t="s">
-        <v>193</v>
-      </c>
-      <c r="C187">
-        <v>2010</v>
       </c>
       <c r="D187">
         <v>9999</v>
@@ -5098,49 +5140,49 @@
         <v>142</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>194</v>
+        <v>25</v>
       </c>
       <c r="B188" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C188">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="D188">
         <v>9999</v>
       </c>
       <c r="E188" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B189" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="C189">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="D189">
         <v>9999</v>
       </c>
       <c r="E189" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>198</v>
+        <v>25</v>
       </c>
       <c r="B190" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="C190">
-        <v>2013</v>
+        <v>2010</v>
       </c>
       <c r="D190">
         <v>9999</v>
@@ -5149,15 +5191,15 @@
         <v>142</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B191" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C191">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="D191">
         <v>9999</v>
@@ -5166,32 +5208,32 @@
         <v>142</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>25</v>
+        <v>195</v>
       </c>
       <c r="B192" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C192">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="D192">
         <v>9999</v>
       </c>
       <c r="E192" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="B193" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="C193">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="D193">
         <v>9999</v>
@@ -5200,49 +5242,49 @@
         <v>142</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>25</v>
+        <v>199</v>
       </c>
       <c r="B194" t="s">
-        <v>349</v>
+        <v>200</v>
       </c>
       <c r="C194">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="D194">
         <v>9999</v>
       </c>
       <c r="E194" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>25</v>
       </c>
       <c r="B195" t="s">
-        <v>350</v>
+        <v>201</v>
       </c>
       <c r="C195">
-        <v>2017</v>
+        <v>2014</v>
       </c>
       <c r="D195">
         <v>9999</v>
       </c>
       <c r="E195" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>258</v>
+        <v>202</v>
       </c>
       <c r="B196" t="s">
-        <v>259</v>
+        <v>203</v>
       </c>
       <c r="C196">
-        <v>2018</v>
+        <v>2015</v>
       </c>
       <c r="D196">
         <v>9999</v>
@@ -5251,15 +5293,15 @@
         <v>142</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>260</v>
+        <v>366</v>
       </c>
       <c r="B197" t="s">
-        <v>261</v>
+        <v>367</v>
       </c>
       <c r="C197">
-        <v>2018</v>
+        <v>2015</v>
       </c>
       <c r="D197">
         <v>9999</v>
@@ -5268,54 +5310,122 @@
         <v>142</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
+        <v>25</v>
+      </c>
+      <c r="B198" t="s">
+        <v>343</v>
+      </c>
+      <c r="C198">
+        <v>2016</v>
+      </c>
+      <c r="D198">
+        <v>9999</v>
+      </c>
+      <c r="E198" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>25</v>
+      </c>
+      <c r="B199" t="s">
+        <v>344</v>
+      </c>
+      <c r="C199">
+        <v>2017</v>
+      </c>
+      <c r="D199">
+        <v>9999</v>
+      </c>
+      <c r="E199" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>256</v>
+      </c>
+      <c r="B200" t="s">
+        <v>257</v>
+      </c>
+      <c r="C200">
+        <v>2018</v>
+      </c>
+      <c r="D200">
+        <v>9999</v>
+      </c>
+      <c r="E200" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>258</v>
+      </c>
+      <c r="B201" t="s">
+        <v>259</v>
+      </c>
+      <c r="C201">
+        <v>2018</v>
+      </c>
+      <c r="D201">
+        <v>9999</v>
+      </c>
+      <c r="E201" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>204</v>
+      </c>
+      <c r="B202" t="s">
         <v>205</v>
       </c>
-      <c r="B198" t="s">
+      <c r="C202">
+        <v>2018</v>
+      </c>
+      <c r="D202">
+        <v>9999</v>
+      </c>
+      <c r="E202" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>260</v>
+      </c>
+      <c r="B203" t="s">
         <v>206</v>
       </c>
-      <c r="C198">
-        <v>2018</v>
-      </c>
-      <c r="D198">
-        <v>9999</v>
-      </c>
-      <c r="E198" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
+      <c r="C203">
+        <v>2019</v>
+      </c>
+      <c r="D203">
+        <v>9999</v>
+      </c>
+      <c r="E203" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>261</v>
+      </c>
+      <c r="B204" t="s">
         <v>262</v>
       </c>
-      <c r="B199" t="s">
-        <v>207</v>
-      </c>
-      <c r="C199">
-        <v>2019</v>
-      </c>
-      <c r="D199">
-        <v>9999</v>
-      </c>
-      <c r="E199" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
-        <v>263</v>
-      </c>
-      <c r="B200" t="s">
-        <v>264</v>
-      </c>
-      <c r="C200">
+      <c r="C204">
         <v>2021</v>
       </c>
-      <c r="D200">
-        <v>9999</v>
-      </c>
-      <c r="E200" t="s">
+      <c r="D204">
+        <v>9999</v>
+      </c>
+      <c r="E204" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Spreadsheets to accompany new SVGs from Ken: 6/15/2021 @ 6:20 a.m.
</commit_message>
<xml_diff>
--- a/xlsx/feature_timeline.xlsx
+++ b/xlsx/feature_timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8376B9-38A6-4B98-9A72-976044AF2502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33620BC1-FF34-44DF-A2C6-D3988CEE9AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="441">
   <si>
     <t>layer_name</t>
   </si>
@@ -1105,18 +1105,12 @@
     <t>Boston &amp; Worcester Railroad (Northborough-Worcester)</t>
   </si>
   <si>
-    <t>1866-w</t>
-  </si>
-  <si>
     <t>South Shore RR (Braintree-Cohasset)</t>
   </si>
   <si>
     <t>South Shore RR (Cohasset-Greenbush)</t>
   </si>
   <si>
-    <t>1872-h</t>
-  </si>
-  <si>
     <t>Eastern RR Essex Branch (Hamilton/Wenham Station-Essex)</t>
   </si>
   <si>
@@ -1325,6 +1319,30 @@
   </si>
   <si>
     <t>Green Line (Lechmere-Medford &amp; Union Square, Somerville)</t>
+  </si>
+  <si>
+    <t>year-1862</t>
+  </si>
+  <si>
+    <t>year-1866-w</t>
+  </si>
+  <si>
+    <t>year-1866</t>
+  </si>
+  <si>
+    <t>year-1854</t>
+  </si>
+  <si>
+    <t>year-1871</t>
+  </si>
+  <si>
+    <t>year-1872-h</t>
+  </si>
+  <si>
+    <t>year-1872</t>
+  </si>
+  <si>
+    <t>year-1873</t>
   </si>
 </sst>
 </file>
@@ -2174,8 +2192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E244" sqref="E244"/>
+    <sheetView tabSelected="1" topLeftCell="A216" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="6" x14ac:dyDescent="0.25"/>
@@ -2570,7 +2588,7 @@
         <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C25">
         <v>1935</v>
@@ -2587,7 +2605,7 @@
         <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C26">
         <v>1953</v>
@@ -2686,10 +2704,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B32" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C32">
         <v>1836</v>
@@ -2859,7 +2877,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C42">
         <v>1933</v>
@@ -2924,10 +2942,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B46" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C46">
         <v>1846</v>
@@ -3080,7 +3098,7 @@
         <v>338</v>
       </c>
       <c r="B55" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C55">
         <v>1849</v>
@@ -3297,8 +3315,8 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
-        <v>1854</v>
+      <c r="A68" s="1" t="s">
+        <v>436</v>
       </c>
       <c r="B68" t="s">
         <v>330</v>
@@ -3365,8 +3383,8 @@
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
-        <v>1862</v>
+      <c r="A72" s="1" t="s">
+        <v>433</v>
       </c>
       <c r="B72" t="s">
         <v>349</v>
@@ -3383,7 +3401,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>361</v>
+        <v>434</v>
       </c>
       <c r="B73" t="s">
         <v>360</v>
@@ -3399,8 +3417,8 @@
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
-        <v>1866</v>
+      <c r="A74" s="1" t="s">
+        <v>435</v>
       </c>
       <c r="B74" t="s">
         <v>281</v>
@@ -3484,11 +3502,11 @@
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
-        <v>1871</v>
+      <c r="A79" s="1" t="s">
+        <v>437</v>
       </c>
       <c r="B79" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C79">
         <v>1871</v>
@@ -3502,10 +3520,10 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>364</v>
+        <v>438</v>
       </c>
       <c r="B80" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C80">
         <v>1872</v>
@@ -3518,8 +3536,8 @@
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="1">
-        <v>1872</v>
+      <c r="A81" s="1" t="s">
+        <v>439</v>
       </c>
       <c r="B81" t="s">
         <v>332</v>
@@ -3535,11 +3553,11 @@
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="1">
-        <v>1873</v>
+      <c r="A82" s="1" t="s">
+        <v>440</v>
       </c>
       <c r="B82" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C82">
         <v>1873</v>
@@ -3692,7 +3710,7 @@
         <v>24</v>
       </c>
       <c r="B91" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C91">
         <v>1894</v>
@@ -4083,7 +4101,7 @@
         <v>24</v>
       </c>
       <c r="B114" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C114">
         <v>1925</v>
@@ -4117,7 +4135,7 @@
         <v>258</v>
       </c>
       <c r="B116" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C116">
         <v>1921</v>
@@ -4131,10 +4149,10 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B117" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C117">
         <v>1923</v>
@@ -4250,10 +4268,10 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B124" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C124">
         <v>1938</v>
@@ -4321,7 +4339,7 @@
         <v>98</v>
       </c>
       <c r="B128" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C128">
         <v>1941</v>
@@ -4355,7 +4373,7 @@
         <v>24</v>
       </c>
       <c r="B130" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C130">
         <v>1947</v>
@@ -4386,10 +4404,10 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B132" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C132">
         <v>1950</v>
@@ -4403,10 +4421,10 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B133" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C133">
         <v>1948</v>
@@ -4420,10 +4438,10 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B134" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C134">
         <v>1941</v>
@@ -4440,7 +4458,7 @@
         <v>102</v>
       </c>
       <c r="B135" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C135">
         <v>1951</v>
@@ -4471,10 +4489,10 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B137" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C137">
         <v>1952</v>
@@ -4488,10 +4506,10 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B138" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C138">
         <v>1957</v>
@@ -4505,10 +4523,10 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B139" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C139">
         <v>1955</v>
@@ -4522,10 +4540,10 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B140" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C140">
         <v>1953</v>
@@ -4573,10 +4591,10 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B143" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C143">
         <v>1955</v>
@@ -4593,7 +4611,7 @@
         <v>107</v>
       </c>
       <c r="B144" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C144">
         <v>1954</v>
@@ -4627,7 +4645,7 @@
         <v>260</v>
       </c>
       <c r="B146" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C146">
         <v>1952</v>
@@ -4644,7 +4662,7 @@
         <v>110</v>
       </c>
       <c r="B147" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C147">
         <v>1954</v>
@@ -4658,10 +4676,10 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B148" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C148">
         <v>1967</v>
@@ -4675,10 +4693,10 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B149" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C149">
         <v>1961</v>
@@ -4692,10 +4710,10 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B150" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C150">
         <v>1955</v>
@@ -4712,7 +4730,7 @@
         <v>108</v>
       </c>
       <c r="B151" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C151">
         <v>1954</v>
@@ -4763,7 +4781,7 @@
         <v>113</v>
       </c>
       <c r="B154" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C154">
         <v>1957</v>
@@ -4797,7 +4815,7 @@
         <v>114</v>
       </c>
       <c r="B156" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C156">
         <v>1958</v>
@@ -4814,7 +4832,7 @@
         <v>24</v>
       </c>
       <c r="B157" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C157">
         <v>1886</v>
@@ -4828,10 +4846,10 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B158" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C158">
         <v>1958</v>
@@ -4848,7 +4866,7 @@
         <v>201</v>
       </c>
       <c r="B159" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C159">
         <v>1959</v>
@@ -4933,7 +4951,7 @@
         <v>121</v>
       </c>
       <c r="B164" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C164">
         <v>1961</v>
@@ -4950,7 +4968,7 @@
         <v>108</v>
       </c>
       <c r="B165" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C165">
         <v>1961</v>
@@ -4967,7 +4985,7 @@
         <v>236</v>
       </c>
       <c r="B166" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C166">
         <v>1962</v>
@@ -4984,7 +5002,7 @@
         <v>123</v>
       </c>
       <c r="B167" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C167">
         <v>1964</v>
@@ -5018,7 +5036,7 @@
         <v>124</v>
       </c>
       <c r="B169" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C169">
         <v>1964</v>
@@ -5035,7 +5053,7 @@
         <v>125</v>
       </c>
       <c r="B170" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C170">
         <v>1960</v>
@@ -5052,7 +5070,7 @@
         <v>24</v>
       </c>
       <c r="B171" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C171">
         <v>1964</v>
@@ -5069,7 +5087,7 @@
         <v>126</v>
       </c>
       <c r="B172" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C172">
         <v>1965</v>
@@ -5086,7 +5104,7 @@
         <v>262</v>
       </c>
       <c r="B173" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C173">
         <v>1965</v>
@@ -5137,7 +5155,7 @@
         <v>237</v>
       </c>
       <c r="B176" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C176">
         <v>1968</v>
@@ -5154,7 +5172,7 @@
         <v>128</v>
       </c>
       <c r="B177" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C177">
         <v>1969</v>
@@ -5168,10 +5186,10 @@
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B178" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C178">
         <v>1982</v>
@@ -5188,7 +5206,7 @@
         <v>129</v>
       </c>
       <c r="B179" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C179">
         <v>1966</v>
@@ -5205,7 +5223,7 @@
         <v>130</v>
       </c>
       <c r="B180" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C180">
         <v>1970</v>
@@ -5239,7 +5257,7 @@
         <v>132</v>
       </c>
       <c r="B182" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C182">
         <v>1973</v>
@@ -5290,7 +5308,7 @@
         <v>24</v>
       </c>
       <c r="B185" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C185">
         <v>1974</v>
@@ -5497,7 +5515,7 @@
         <v>261</v>
       </c>
       <c r="B197" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C197">
         <v>1987</v>
@@ -6302,7 +6320,7 @@
         <v>245</v>
       </c>
       <c r="B244" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C244">
         <v>2021</v>

</xml_diff>

<commit_message>
Latest spreadsheets from Ken, as of this morning.
</commit_message>
<xml_diff>
--- a/xlsx/feature_timeline.xlsx
+++ b/xlsx/feature_timeline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kend/Documents/General Maps/Time Line/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\historical-transportation-map\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5478A5F2-97D9-2642-B827-572D47E0E6AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5126289-0ECE-4E0C-AF88-02E398B13332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="18460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="feature_timeline" sheetId="1" r:id="rId1"/>
@@ -2228,20 +2228,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
-      <selection activeCell="B165" sqref="B165"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelRow="6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="6" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2275,7 +2275,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2331,7 +2331,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -2387,7 +2387,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -2418,7 +2418,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>328</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>327</v>
       </c>
@@ -2452,7 +2452,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -2690,7 +2690,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -2707,7 +2707,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>342</v>
       </c>
@@ -2724,7 +2724,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>338</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>358</v>
       </c>
@@ -2775,7 +2775,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -2826,7 +2826,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>203</v>
       </c>
@@ -2843,7 +2843,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>202</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>39</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>40</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>343</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>41</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>42</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>384</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>260</v>
       </c>
@@ -3030,7 +3030,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>205</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>43</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>206</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>209</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>208</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>324</v>
       </c>
@@ -3132,7 +3132,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>44</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>326</v>
       </c>
@@ -3166,7 +3166,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>45</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>24</v>
       </c>
@@ -3200,7 +3200,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>46</v>
       </c>
@@ -3217,7 +3217,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>210</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>214</v>
       </c>
@@ -3251,7 +3251,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>335</v>
       </c>
@@ -3268,7 +3268,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>332</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>213</v>
       </c>
@@ -3302,7 +3302,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>330</v>
       </c>
@@ -3319,7 +3319,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>211</v>
       </c>
@@ -3336,7 +3336,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>212</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>224</v>
       </c>
@@ -3370,7 +3370,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>421</v>
       </c>
@@ -3387,7 +3387,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>24</v>
       </c>
@@ -3404,7 +3404,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>49</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>50</v>
       </c>
@@ -3438,7 +3438,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>418</v>
       </c>
@@ -3455,7 +3455,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>419</v>
       </c>
@@ -3472,7 +3472,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>420</v>
       </c>
@@ -3489,7 +3489,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>215</v>
       </c>
@@ -3506,7 +3506,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>51</v>
       </c>
@@ -3523,7 +3523,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>207</v>
       </c>
@@ -3540,7 +3540,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>204</v>
       </c>
@@ -3557,7 +3557,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>422</v>
       </c>
@@ -3574,7 +3574,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>423</v>
       </c>
@@ -3591,7 +3591,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>424</v>
       </c>
@@ -3608,7 +3608,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>425</v>
       </c>
@@ -3619,13 +3619,13 @@
         <v>1873</v>
       </c>
       <c r="D83">
-        <v>9999</v>
+        <v>1977</v>
       </c>
       <c r="E83" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>216</v>
       </c>
@@ -3642,7 +3642,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>217</v>
       </c>
@@ -3659,7 +3659,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>53</v>
       </c>
@@ -3676,7 +3676,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>54</v>
       </c>
@@ -3693,7 +3693,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>55</v>
       </c>
@@ -3710,7 +3710,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>57</v>
       </c>
@@ -3727,7 +3727,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>24</v>
       </c>
@@ -3744,7 +3744,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>24</v>
       </c>
@@ -3761,7 +3761,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>24</v>
       </c>
@@ -3778,7 +3778,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>62</v>
       </c>
@@ -3795,7 +3795,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>64</v>
       </c>
@@ -3812,7 +3812,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>24</v>
       </c>
@@ -3829,7 +3829,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>67</v>
       </c>
@@ -3846,7 +3846,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>68</v>
       </c>
@@ -3863,7 +3863,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>70</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>24</v>
       </c>
@@ -3897,7 +3897,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>72</v>
       </c>
@@ -3914,7 +3914,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>74</v>
       </c>
@@ -3931,7 +3931,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>24</v>
       </c>
@@ -3948,7 +3948,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>220</v>
       </c>
@@ -3965,7 +3965,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>75</v>
       </c>
@@ -3982,7 +3982,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>76</v>
       </c>
@@ -3999,7 +3999,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>24</v>
       </c>
@@ -4016,7 +4016,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>24</v>
       </c>
@@ -4033,7 +4033,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>79</v>
       </c>
@@ -4050,7 +4050,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>80</v>
       </c>
@@ -4067,7 +4067,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>24</v>
       </c>
@@ -4084,7 +4084,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>81</v>
       </c>
@@ -4101,7 +4101,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>225</v>
       </c>
@@ -4118,7 +4118,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>82</v>
       </c>
@@ -4135,7 +4135,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>24</v>
       </c>
@@ -4152,7 +4152,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>84</v>
       </c>
@@ -4169,7 +4169,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>24</v>
       </c>
@@ -4186,7 +4186,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>24</v>
       </c>
@@ -4203,7 +4203,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>86</v>
       </c>
@@ -4220,7 +4220,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>24</v>
       </c>
@@ -4237,7 +4237,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>24</v>
       </c>
@@ -4254,7 +4254,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>48</v>
       </c>
@@ -4271,7 +4271,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>252</v>
       </c>
@@ -4288,7 +4288,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>356</v>
       </c>
@@ -4305,7 +4305,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>89</v>
       </c>
@@ -4322,7 +4322,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>259</v>
       </c>
@@ -4339,7 +4339,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>90</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>24</v>
       </c>
@@ -4373,7 +4373,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>24</v>
       </c>
@@ -4390,7 +4390,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>24</v>
       </c>
@@ -4407,7 +4407,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>24</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>93</v>
       </c>
@@ -4441,7 +4441,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>361</v>
       </c>
@@ -4458,7 +4458,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>24</v>
       </c>
@@ -4475,7 +4475,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>95</v>
       </c>
@@ -4492,7 +4492,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>97</v>
       </c>
@@ -4509,7 +4509,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>98</v>
       </c>
@@ -4526,7 +4526,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>24</v>
       </c>
@@ -4543,7 +4543,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>24</v>
       </c>
@@ -4560,7 +4560,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>100</v>
       </c>
@@ -4577,7 +4577,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>367</v>
       </c>
@@ -4594,7 +4594,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>365</v>
       </c>
@@ -4611,7 +4611,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>363</v>
       </c>
@@ -4628,7 +4628,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>102</v>
       </c>
@@ -4645,7 +4645,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>103</v>
       </c>
@@ -4662,7 +4662,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>370</v>
       </c>
@@ -4679,7 +4679,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>380</v>
       </c>
@@ -4696,7 +4696,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>378</v>
       </c>
@@ -4713,7 +4713,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>371</v>
       </c>
@@ -4730,7 +4730,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>24</v>
       </c>
@@ -4747,7 +4747,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>106</v>
       </c>
@@ -4764,7 +4764,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>377</v>
       </c>
@@ -4781,7 +4781,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>107</v>
       </c>
@@ -4798,7 +4798,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>109</v>
       </c>
@@ -4815,7 +4815,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>253</v>
       </c>
@@ -4832,7 +4832,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>110</v>
       </c>
@@ -4849,7 +4849,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>391</v>
       </c>
@@ -4866,7 +4866,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>376</v>
       </c>
@@ -4883,7 +4883,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>108</v>
       </c>
@@ -4900,7 +4900,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>24</v>
       </c>
@@ -4917,7 +4917,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>24</v>
       </c>
@@ -4934,7 +4934,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>24</v>
       </c>
@@ -4951,7 +4951,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>113</v>
       </c>
@@ -4968,7 +4968,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>256</v>
       </c>
@@ -4985,7 +4985,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>114</v>
       </c>
@@ -5002,7 +5002,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>24</v>
       </c>
@@ -5019,7 +5019,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>383</v>
       </c>
@@ -5036,7 +5036,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>199</v>
       </c>
@@ -5053,7 +5053,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>115</v>
       </c>
@@ -5070,7 +5070,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>24</v>
       </c>
@@ -5087,7 +5087,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>117</v>
       </c>
@@ -5104,7 +5104,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>119</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>121</v>
       </c>
@@ -5138,7 +5138,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>393</v>
       </c>
@@ -5155,7 +5155,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>24</v>
       </c>
@@ -5172,7 +5172,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>233</v>
       </c>
@@ -5189,7 +5189,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>123</v>
       </c>
@@ -5206,7 +5206,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>118</v>
       </c>
@@ -5223,7 +5223,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>24</v>
       </c>
@@ -5240,7 +5240,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>124</v>
       </c>
@@ -5257,7 +5257,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>125</v>
       </c>
@@ -5274,7 +5274,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>24</v>
       </c>
@@ -5291,7 +5291,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>126</v>
       </c>
@@ -5308,7 +5308,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>255</v>
       </c>
@@ -5325,7 +5325,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>127</v>
       </c>
@@ -5342,7 +5342,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>24</v>
       </c>
@@ -5359,7 +5359,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>234</v>
       </c>
@@ -5376,7 +5376,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>128</v>
       </c>
@@ -5393,7 +5393,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>394</v>
       </c>
@@ -5410,7 +5410,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>129</v>
       </c>
@@ -5427,7 +5427,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>130</v>
       </c>
@@ -5444,7 +5444,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>131</v>
       </c>
@@ -5461,7 +5461,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>132</v>
       </c>
@@ -5478,7 +5478,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>24</v>
       </c>
@@ -5495,7 +5495,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>24</v>
       </c>
@@ -5512,7 +5512,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>24</v>
       </c>
@@ -5529,7 +5529,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>133</v>
       </c>
@@ -5546,7 +5546,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>24</v>
       </c>
@@ -5563,7 +5563,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>122</v>
       </c>
@@ -5580,7 +5580,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>137</v>
       </c>
@@ -5597,7 +5597,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>138</v>
       </c>
@@ -5614,7 +5614,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>24</v>
       </c>
@@ -5631,7 +5631,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>140</v>
       </c>
@@ -5648,7 +5648,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>24</v>
       </c>
@@ -5665,7 +5665,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>141</v>
       </c>
@@ -5682,7 +5682,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>142</v>
       </c>
@@ -5699,7 +5699,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>143</v>
       </c>
@@ -5716,7 +5716,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>145</v>
       </c>
@@ -5733,7 +5733,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>254</v>
       </c>
@@ -5750,7 +5750,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>146</v>
       </c>
@@ -5767,7 +5767,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>148</v>
       </c>
@@ -5784,7 +5784,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>24</v>
       </c>
@@ -5801,7 +5801,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>24</v>
       </c>
@@ -5818,7 +5818,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>152</v>
       </c>
@@ -5835,7 +5835,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>24</v>
       </c>
@@ -5852,7 +5852,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="215" spans="1:6" ht="15" customHeight="1" outlineLevel="6" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:6" ht="15" customHeight="1" outlineLevel="6" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>153</v>
       </c>
@@ -5869,7 +5869,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>24</v>
       </c>
@@ -5886,7 +5886,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>156</v>
       </c>
@@ -5906,7 +5906,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>24</v>
       </c>
@@ -5923,7 +5923,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>158</v>
       </c>
@@ -5943,7 +5943,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>159</v>
       </c>
@@ -5963,7 +5963,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>160</v>
       </c>
@@ -5980,7 +5980,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>24</v>
       </c>
@@ -5997,7 +5997,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>218</v>
       </c>
@@ -6014,7 +6014,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>163</v>
       </c>
@@ -6031,7 +6031,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>165</v>
       </c>
@@ -6048,7 +6048,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>24</v>
       </c>
@@ -6065,7 +6065,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>221</v>
       </c>
@@ -6082,7 +6082,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>24</v>
       </c>
@@ -6099,7 +6099,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>170</v>
       </c>
@@ -6116,7 +6116,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>24</v>
       </c>
@@ -6133,7 +6133,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>24</v>
       </c>
@@ -6150,7 +6150,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>235</v>
       </c>
@@ -6167,7 +6167,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>173</v>
       </c>
@@ -6184,7 +6184,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>175</v>
       </c>
@@ -6204,7 +6204,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>177</v>
       </c>
@@ -6221,7 +6221,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>24</v>
       </c>
@@ -6238,7 +6238,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>180</v>
       </c>
@@ -6255,7 +6255,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>24</v>
       </c>
@@ -6272,7 +6272,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>183</v>
       </c>
@@ -6289,7 +6289,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>24</v>
       </c>
@@ -6306,7 +6306,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>185</v>
       </c>
@@ -6323,7 +6323,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>187</v>
       </c>
@@ -6340,7 +6340,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>189</v>
       </c>
@@ -6357,7 +6357,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>191</v>
       </c>
@@ -6374,7 +6374,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>24</v>
       </c>
@@ -6391,7 +6391,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>194</v>
       </c>
@@ -6408,7 +6408,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>263</v>
       </c>
@@ -6425,7 +6425,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>261</v>
       </c>
@@ -6442,7 +6442,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>24</v>
       </c>
@@ -6459,7 +6459,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>24</v>
       </c>
@@ -6476,7 +6476,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>236</v>
       </c>
@@ -6493,7 +6493,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>238</v>
       </c>
@@ -6510,7 +6510,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>196</v>
       </c>
@@ -6527,7 +6527,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>240</v>
       </c>
@@ -6544,7 +6544,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>241</v>
       </c>

</xml_diff>

<commit_message>
Opening date of GLX is 2022, not 2021.
</commit_message>
<xml_diff>
--- a/xlsx/feature_timeline.xlsx
+++ b/xlsx/feature_timeline.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\historical-transportation-map\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9F2718-E337-4AC2-8C47-70BD9B78EA3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3696F8B4-884B-4317-969A-4FCD004F67DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -736,9 +736,6 @@
     <t>MCRT-2019</t>
   </si>
   <si>
-    <t>Green_Line-2021</t>
-  </si>
-  <si>
     <t>Nashua &amp; Lowell Railroad</t>
   </si>
   <si>
@@ -1553,6 +1550,9 @@
   </si>
   <si>
     <t>Green Line (Heath Street-Forest Hills)</t>
+  </si>
+  <si>
+    <t>Green_Line-2022</t>
   </si>
 </sst>
 </file>
@@ -2036,12 +2036,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2402,8 +2401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F311"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D102" sqref="D102"/>
+    <sheetView tabSelected="1" topLeftCell="A286" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C311" sqref="C311"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="6" x14ac:dyDescent="0.25"/>
@@ -2594,10 +2593,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B13" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C13">
         <v>1805</v>
@@ -2611,10 +2610,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B14" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C14">
         <v>1805</v>
@@ -2631,7 +2630,7 @@
         <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C15">
         <v>1806</v>
@@ -2716,7 +2715,7 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C20">
         <v>1811</v>
@@ -2733,7 +2732,7 @@
         <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C21">
         <v>1817</v>
@@ -2750,7 +2749,7 @@
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C22">
         <v>1822</v>
@@ -2818,7 +2817,7 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C26">
         <v>1935</v>
@@ -2835,7 +2834,7 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C27">
         <v>1953</v>
@@ -2852,7 +2851,7 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C28">
         <v>1834</v>
@@ -2869,7 +2868,7 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C29">
         <v>1834</v>
@@ -2883,10 +2882,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B30" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C30">
         <v>1835</v>
@@ -2900,10 +2899,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>325</v>
+      </c>
+      <c r="B31" t="s">
         <v>326</v>
-      </c>
-      <c r="B31" t="s">
-        <v>327</v>
       </c>
       <c r="C31">
         <v>1835</v>
@@ -2920,7 +2919,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C32">
         <v>1835</v>
@@ -2934,10 +2933,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B33" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C33">
         <v>1836</v>
@@ -2954,7 +2953,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C34">
         <v>1836</v>
@@ -2971,7 +2970,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C35">
         <v>1925</v>
@@ -2988,7 +2987,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C36">
         <v>1838</v>
@@ -3005,7 +3004,7 @@
         <v>200</v>
       </c>
       <c r="B37" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C37">
         <v>1838</v>
@@ -3022,7 +3021,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C38">
         <v>1839</v>
@@ -3039,7 +3038,7 @@
         <v>24</v>
       </c>
       <c r="B39" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C39">
         <v>1839</v>
@@ -3056,7 +3055,7 @@
         <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C40">
         <v>1840</v>
@@ -3073,7 +3072,7 @@
         <v>38</v>
       </c>
       <c r="B41" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C41">
         <v>1843</v>
@@ -3090,7 +3089,7 @@
         <v>199</v>
       </c>
       <c r="B42" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C42">
         <v>1844</v>
@@ -3107,7 +3106,7 @@
         <v>39</v>
       </c>
       <c r="B43" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C43">
         <v>1844</v>
@@ -3124,7 +3123,7 @@
         <v>40</v>
       </c>
       <c r="B44" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C44">
         <v>1933</v>
@@ -3138,10 +3137,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B45" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C45">
         <v>1845</v>
@@ -3158,7 +3157,7 @@
         <v>41</v>
       </c>
       <c r="B46" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C46">
         <v>1845</v>
@@ -3175,7 +3174,7 @@
         <v>42</v>
       </c>
       <c r="B47" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C47">
         <v>1845</v>
@@ -3189,10 +3188,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>360</v>
+      </c>
+      <c r="B48" t="s">
         <v>361</v>
-      </c>
-      <c r="B48" t="s">
-        <v>362</v>
       </c>
       <c r="C48">
         <v>1846</v>
@@ -3209,7 +3208,7 @@
         <v>24</v>
       </c>
       <c r="B49" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C49">
         <v>1846</v>
@@ -3226,7 +3225,7 @@
         <v>24</v>
       </c>
       <c r="B50" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C50">
         <v>1866</v>
@@ -3240,10 +3239,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B51" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C51">
         <v>1866</v>
@@ -3260,7 +3259,7 @@
         <v>202</v>
       </c>
       <c r="B52" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C52">
         <v>1846</v>
@@ -3277,7 +3276,7 @@
         <v>43</v>
       </c>
       <c r="B53" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C53">
         <v>1847</v>
@@ -3294,7 +3293,7 @@
         <v>203</v>
       </c>
       <c r="B54" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C54">
         <v>1848</v>
@@ -3311,7 +3310,7 @@
         <v>206</v>
       </c>
       <c r="B55" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C55">
         <v>1847</v>
@@ -3328,7 +3327,7 @@
         <v>24</v>
       </c>
       <c r="B56" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C56">
         <v>1847</v>
@@ -3345,7 +3344,7 @@
         <v>24</v>
       </c>
       <c r="B57" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C57">
         <v>1847</v>
@@ -3362,7 +3361,7 @@
         <v>24</v>
       </c>
       <c r="B58" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C58">
         <v>1847</v>
@@ -3379,7 +3378,7 @@
         <v>24</v>
       </c>
       <c r="B59" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C59">
         <v>1847</v>
@@ -3396,7 +3395,7 @@
         <v>24</v>
       </c>
       <c r="B60" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C60">
         <v>1847</v>
@@ -3413,7 +3412,7 @@
         <v>205</v>
       </c>
       <c r="B61" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C61">
         <v>1848</v>
@@ -3427,10 +3426,10 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B62" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C62">
         <v>1848</v>
@@ -3447,7 +3446,7 @@
         <v>24</v>
       </c>
       <c r="B63" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C63">
         <v>1848</v>
@@ -3464,7 +3463,7 @@
         <v>24</v>
       </c>
       <c r="B64" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C64">
         <v>1848</v>
@@ -3481,7 +3480,7 @@
         <v>24</v>
       </c>
       <c r="B65" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C65">
         <v>1848</v>
@@ -3498,7 +3497,7 @@
         <v>44</v>
       </c>
       <c r="B66" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C66">
         <v>1849</v>
@@ -3512,15 +3511,15 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B67" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C67">
         <v>1849</v>
       </c>
-      <c r="D67" s="3">
+      <c r="D67" s="2">
         <v>1959</v>
       </c>
       <c r="E67" t="s">
@@ -3532,7 +3531,7 @@
         <v>45</v>
       </c>
       <c r="B68" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C68">
         <v>1849</v>
@@ -3549,7 +3548,7 @@
         <v>24</v>
       </c>
       <c r="B69" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C69">
         <v>1849</v>
@@ -3566,7 +3565,7 @@
         <v>24</v>
       </c>
       <c r="B70" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C70">
         <v>1849</v>
@@ -3583,7 +3582,7 @@
         <v>24</v>
       </c>
       <c r="B71" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C71">
         <v>1849</v>
@@ -3600,7 +3599,7 @@
         <v>46</v>
       </c>
       <c r="B72" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C72">
         <v>1850</v>
@@ -3634,7 +3633,7 @@
         <v>211</v>
       </c>
       <c r="B74" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C74">
         <v>1855</v>
@@ -3648,10 +3647,10 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B75" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C75">
         <v>1850</v>
@@ -3665,10 +3664,10 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B76" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C76">
         <v>1851</v>
@@ -3685,7 +3684,7 @@
         <v>24</v>
       </c>
       <c r="B77" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C77">
         <v>1851</v>
@@ -3702,7 +3701,7 @@
         <v>210</v>
       </c>
       <c r="B78" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C78">
         <v>1854</v>
@@ -3716,10 +3715,10 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B79" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C79">
         <v>1850</v>
@@ -3736,7 +3735,7 @@
         <v>24</v>
       </c>
       <c r="B80" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C80">
         <v>1852</v>
@@ -3753,7 +3752,7 @@
         <v>208</v>
       </c>
       <c r="B81" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C81">
         <v>1853</v>
@@ -3770,7 +3769,7 @@
         <v>209</v>
       </c>
       <c r="B82" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C82">
         <v>1855</v>
@@ -3787,7 +3786,7 @@
         <v>221</v>
       </c>
       <c r="B83" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C83">
         <v>1861</v>
@@ -3801,10 +3800,10 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B84" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C84">
         <v>1854</v>
@@ -3821,7 +3820,7 @@
         <v>24</v>
       </c>
       <c r="B85" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C85">
         <v>1855</v>
@@ -3838,7 +3837,7 @@
         <v>24</v>
       </c>
       <c r="B86" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C86">
         <v>1856</v>
@@ -3855,7 +3854,7 @@
         <v>49</v>
       </c>
       <c r="B87" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C87">
         <v>1861</v>
@@ -3872,7 +3871,7 @@
         <v>50</v>
       </c>
       <c r="B88" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C88">
         <v>1861</v>
@@ -3889,7 +3888,7 @@
         <v>24</v>
       </c>
       <c r="B89" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C89">
         <v>1862</v>
@@ -3903,10 +3902,10 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B90" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C90">
         <v>1863</v>
@@ -3920,10 +3919,10 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B91" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C91">
         <v>1866</v>
@@ -3937,10 +3936,10 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B92" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C92">
         <v>1866</v>
@@ -3957,7 +3956,7 @@
         <v>212</v>
       </c>
       <c r="B93" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C93">
         <v>1870</v>
@@ -3991,7 +3990,7 @@
         <v>204</v>
       </c>
       <c r="B95" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C95">
         <v>1883</v>
@@ -4008,7 +4007,7 @@
         <v>201</v>
       </c>
       <c r="B96" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C96">
         <v>1868</v>
@@ -4022,10 +4021,10 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B97" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C97">
         <v>1871</v>
@@ -4039,10 +4038,10 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B98" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C98">
         <v>1872</v>
@@ -4056,10 +4055,10 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B99" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C99">
         <v>1872</v>
@@ -4073,10 +4072,10 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B100" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C100">
         <v>1873</v>
@@ -4093,7 +4092,7 @@
         <v>24</v>
       </c>
       <c r="B101" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C101">
         <v>1873</v>
@@ -4106,11 +4105,11 @@
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="2" t="s">
+      <c r="A102" t="s">
         <v>213</v>
       </c>
       <c r="B102" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C102">
         <v>1871</v>
@@ -4127,7 +4126,7 @@
         <v>24</v>
       </c>
       <c r="B103" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C103">
         <v>1874</v>
@@ -4144,7 +4143,7 @@
         <v>214</v>
       </c>
       <c r="B104" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C104">
         <v>1874</v>
@@ -4161,7 +4160,7 @@
         <v>24</v>
       </c>
       <c r="B105" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C105">
         <v>1875</v>
@@ -4178,7 +4177,7 @@
         <v>24</v>
       </c>
       <c r="B106" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C106">
         <v>1876</v>
@@ -4195,7 +4194,7 @@
         <v>24</v>
       </c>
       <c r="B107" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C107">
         <v>1879</v>
@@ -4212,7 +4211,7 @@
         <v>24</v>
       </c>
       <c r="B108" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C108">
         <v>1880</v>
@@ -4229,7 +4228,7 @@
         <v>53</v>
       </c>
       <c r="B109" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C109">
         <v>1881</v>
@@ -4246,7 +4245,7 @@
         <v>24</v>
       </c>
       <c r="B110" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C110">
         <v>1881</v>
@@ -4263,7 +4262,7 @@
         <v>24</v>
       </c>
       <c r="B111" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C111">
         <v>1885</v>
@@ -4280,7 +4279,7 @@
         <v>54</v>
       </c>
       <c r="B112" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C112">
         <v>1845</v>
@@ -4297,7 +4296,7 @@
         <v>55</v>
       </c>
       <c r="B113" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C113">
         <v>1889</v>
@@ -4331,7 +4330,7 @@
         <v>24</v>
       </c>
       <c r="B115" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C115">
         <v>1890</v>
@@ -4348,7 +4347,7 @@
         <v>24</v>
       </c>
       <c r="B116" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C116">
         <v>1890</v>
@@ -4365,7 +4364,7 @@
         <v>24</v>
       </c>
       <c r="B117" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C117">
         <v>1892</v>
@@ -4382,7 +4381,7 @@
         <v>24</v>
       </c>
       <c r="B118" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C118">
         <v>1892</v>
@@ -4433,7 +4432,7 @@
         <v>24</v>
       </c>
       <c r="B121" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C121">
         <v>1894</v>
@@ -4484,7 +4483,7 @@
         <v>24</v>
       </c>
       <c r="B124" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C124">
         <v>1888</v>
@@ -4518,7 +4517,7 @@
         <v>66</v>
       </c>
       <c r="B126" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C126">
         <v>1901</v>
@@ -4552,7 +4551,7 @@
         <v>69</v>
       </c>
       <c r="B128" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C128">
         <v>1901</v>
@@ -4569,7 +4568,7 @@
         <v>24</v>
       </c>
       <c r="B129" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C129">
         <v>1901</v>
@@ -4603,7 +4602,7 @@
         <v>72</v>
       </c>
       <c r="B131" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C131">
         <v>1906</v>
@@ -4620,7 +4619,7 @@
         <v>24</v>
       </c>
       <c r="B132" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C132">
         <v>9999</v>
@@ -4637,7 +4636,7 @@
         <v>24</v>
       </c>
       <c r="B133" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C133">
         <v>1908</v>
@@ -4654,7 +4653,7 @@
         <v>217</v>
       </c>
       <c r="B134" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C134">
         <v>1909</v>
@@ -4671,7 +4670,7 @@
         <v>73</v>
       </c>
       <c r="B135" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C135">
         <v>1912</v>
@@ -4722,7 +4721,7 @@
         <v>24</v>
       </c>
       <c r="B138" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C138">
         <v>1912</v>
@@ -4739,7 +4738,7 @@
         <v>77</v>
       </c>
       <c r="B139" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C139">
         <v>1914</v>
@@ -4756,7 +4755,7 @@
         <v>78</v>
       </c>
       <c r="B140" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C140">
         <v>1915</v>
@@ -4773,7 +4772,7 @@
         <v>24</v>
       </c>
       <c r="B141" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C141">
         <v>1916</v>
@@ -4790,7 +4789,7 @@
         <v>79</v>
       </c>
       <c r="B142" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C142">
         <v>1916</v>
@@ -4807,7 +4806,7 @@
         <v>222</v>
       </c>
       <c r="B143" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C143">
         <v>1917</v>
@@ -4824,7 +4823,7 @@
         <v>80</v>
       </c>
       <c r="B144" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C144">
         <v>1918</v>
@@ -4858,7 +4857,7 @@
         <v>82</v>
       </c>
       <c r="B146" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C146">
         <v>1919</v>
@@ -4875,7 +4874,7 @@
         <v>24</v>
       </c>
       <c r="B147" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C147">
         <v>1921</v>
@@ -4926,7 +4925,7 @@
         <v>24</v>
       </c>
       <c r="B150" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C150">
         <v>1923</v>
@@ -4943,7 +4942,7 @@
         <v>24</v>
       </c>
       <c r="B151" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C151">
         <v>1924</v>
@@ -4960,7 +4959,7 @@
         <v>48</v>
       </c>
       <c r="B152" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C152">
         <v>1933</v>
@@ -4974,10 +4973,10 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B153" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C153">
         <v>1921</v>
@@ -4991,10 +4990,10 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B154" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C154">
         <v>1923</v>
@@ -5011,7 +5010,7 @@
         <v>87</v>
       </c>
       <c r="B155" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C155">
         <v>1927</v>
@@ -5025,10 +5024,10 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B156" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C156">
         <v>1928</v>
@@ -5096,7 +5095,7 @@
         <v>24</v>
       </c>
       <c r="B160" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C160">
         <v>1932</v>
@@ -5113,7 +5112,7 @@
         <v>24</v>
       </c>
       <c r="B161" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C161">
         <v>1932</v>
@@ -5130,7 +5129,7 @@
         <v>24</v>
       </c>
       <c r="B162" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C162">
         <v>1932</v>
@@ -5161,10 +5160,10 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
+        <v>340</v>
+      </c>
+      <c r="B164" t="s">
         <v>341</v>
-      </c>
-      <c r="B164" t="s">
-        <v>342</v>
       </c>
       <c r="C164">
         <v>1938</v>
@@ -5181,7 +5180,7 @@
         <v>24</v>
       </c>
       <c r="B165" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C165">
         <v>1936</v>
@@ -5215,7 +5214,7 @@
         <v>95</v>
       </c>
       <c r="B167" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C167">
         <v>1941</v>
@@ -5232,7 +5231,7 @@
         <v>96</v>
       </c>
       <c r="B168" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C168">
         <v>1941</v>
@@ -5266,7 +5265,7 @@
         <v>24</v>
       </c>
       <c r="B170" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C170">
         <v>1947</v>
@@ -5297,10 +5296,10 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
+        <v>346</v>
+      </c>
+      <c r="B172" t="s">
         <v>347</v>
-      </c>
-      <c r="B172" t="s">
-        <v>348</v>
       </c>
       <c r="C172">
         <v>1950</v>
@@ -5314,10 +5313,10 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
+        <v>344</v>
+      </c>
+      <c r="B173" t="s">
         <v>345</v>
-      </c>
-      <c r="B173" t="s">
-        <v>346</v>
       </c>
       <c r="C173">
         <v>1948</v>
@@ -5331,10 +5330,10 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
+        <v>342</v>
+      </c>
+      <c r="B174" t="s">
         <v>343</v>
-      </c>
-      <c r="B174" t="s">
-        <v>344</v>
       </c>
       <c r="C174">
         <v>1941</v>
@@ -5351,7 +5350,7 @@
         <v>100</v>
       </c>
       <c r="B175" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C175">
         <v>1951</v>
@@ -5382,10 +5381,10 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B177" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C177">
         <v>1952</v>
@@ -5402,7 +5401,7 @@
         <v>24</v>
       </c>
       <c r="B178" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C178">
         <v>9999</v>
@@ -5419,7 +5418,7 @@
         <v>24</v>
       </c>
       <c r="B179" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C179">
         <v>9999</v>
@@ -5436,7 +5435,7 @@
         <v>24</v>
       </c>
       <c r="B180" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C180">
         <v>9999</v>
@@ -5453,7 +5452,7 @@
         <v>24</v>
       </c>
       <c r="B181" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C181">
         <v>9999</v>
@@ -5470,7 +5469,7 @@
         <v>24</v>
       </c>
       <c r="B182" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C182">
         <v>9999</v>
@@ -5487,7 +5486,7 @@
         <v>24</v>
       </c>
       <c r="B183" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C183">
         <v>9999</v>
@@ -5504,7 +5503,7 @@
         <v>24</v>
       </c>
       <c r="B184" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C184">
         <v>9999</v>
@@ -5521,7 +5520,7 @@
         <v>24</v>
       </c>
       <c r="B185" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C185">
         <v>9999</v>
@@ -5538,7 +5537,7 @@
         <v>24</v>
       </c>
       <c r="B186" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C186">
         <v>9999</v>
@@ -5552,10 +5551,10 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
+        <v>357</v>
+      </c>
+      <c r="B187" t="s">
         <v>358</v>
-      </c>
-      <c r="B187" t="s">
-        <v>359</v>
       </c>
       <c r="C187">
         <v>1957</v>
@@ -5569,10 +5568,10 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
+        <v>355</v>
+      </c>
+      <c r="B188" t="s">
         <v>356</v>
-      </c>
-      <c r="B188" t="s">
-        <v>357</v>
       </c>
       <c r="C188">
         <v>1955</v>
@@ -5586,10 +5585,10 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
+        <v>350</v>
+      </c>
+      <c r="B189" t="s">
         <v>351</v>
-      </c>
-      <c r="B189" t="s">
-        <v>352</v>
       </c>
       <c r="C189">
         <v>1953</v>
@@ -5623,7 +5622,7 @@
         <v>104</v>
       </c>
       <c r="B191" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C191">
         <v>1952</v>
@@ -5637,10 +5636,10 @@
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B192" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C192">
         <v>1955</v>
@@ -5657,7 +5656,7 @@
         <v>105</v>
       </c>
       <c r="B193" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C193">
         <v>1954</v>
@@ -5674,7 +5673,7 @@
         <v>107</v>
       </c>
       <c r="B194" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C194">
         <v>1954</v>
@@ -5688,10 +5687,10 @@
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B195" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C195">
         <v>1952</v>
@@ -5708,7 +5707,7 @@
         <v>24</v>
       </c>
       <c r="B196" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C196">
         <v>1953</v>
@@ -5722,10 +5721,10 @@
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
+        <v>472</v>
+      </c>
+      <c r="B197" t="s">
         <v>473</v>
-      </c>
-      <c r="B197" t="s">
-        <v>474</v>
       </c>
       <c r="C197">
         <v>1954</v>
@@ -5742,7 +5741,7 @@
         <v>108</v>
       </c>
       <c r="B198" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C198">
         <v>1954</v>
@@ -5756,10 +5755,10 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
+        <v>367</v>
+      </c>
+      <c r="B199" t="s">
         <v>368</v>
-      </c>
-      <c r="B199" t="s">
-        <v>369</v>
       </c>
       <c r="C199">
         <v>1967</v>
@@ -5773,10 +5772,10 @@
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B200" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C200">
         <v>1955</v>
@@ -5793,7 +5792,7 @@
         <v>106</v>
       </c>
       <c r="B201" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C201">
         <v>1954</v>
@@ -5827,7 +5826,7 @@
         <v>24</v>
       </c>
       <c r="B203" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C203">
         <v>1956</v>
@@ -5861,7 +5860,7 @@
         <v>24</v>
       </c>
       <c r="B205" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C205">
         <v>1955</v>
@@ -5878,7 +5877,7 @@
         <v>111</v>
       </c>
       <c r="B206" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C206">
         <v>1957</v>
@@ -5892,10 +5891,10 @@
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
+        <v>475</v>
+      </c>
+      <c r="B207" t="s">
         <v>476</v>
-      </c>
-      <c r="B207" t="s">
-        <v>477</v>
       </c>
       <c r="C207">
         <v>1955</v>
@@ -5909,10 +5908,10 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
+        <v>251</v>
+      </c>
+      <c r="B208" t="s">
         <v>252</v>
-      </c>
-      <c r="B208" t="s">
-        <v>253</v>
       </c>
       <c r="C208">
         <v>1961</v>
@@ -5929,7 +5928,7 @@
         <v>24</v>
       </c>
       <c r="B209" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C209">
         <v>1958</v>
@@ -5946,7 +5945,7 @@
         <v>112</v>
       </c>
       <c r="B210" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C210">
         <v>1958</v>
@@ -5963,7 +5962,7 @@
         <v>24</v>
       </c>
       <c r="B211" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C211">
         <v>1886</v>
@@ -5977,10 +5976,10 @@
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
+        <v>467</v>
+      </c>
+      <c r="B212" t="s">
         <v>468</v>
-      </c>
-      <c r="B212" t="s">
-        <v>469</v>
       </c>
       <c r="C212">
         <v>1958</v>
@@ -5994,10 +5993,10 @@
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B213" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C213">
         <v>1958</v>
@@ -6014,7 +6013,7 @@
         <v>196</v>
       </c>
       <c r="B214" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C214">
         <v>1959</v>
@@ -6031,7 +6030,7 @@
         <v>113</v>
       </c>
       <c r="B215" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C215">
         <v>1959</v>
@@ -6065,7 +6064,7 @@
         <v>115</v>
       </c>
       <c r="B217" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C217">
         <v>1959</v>
@@ -6099,7 +6098,7 @@
         <v>119</v>
       </c>
       <c r="B219" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C219">
         <v>1961</v>
@@ -6113,10 +6112,10 @@
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B220" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C220">
         <v>1961</v>
@@ -6133,7 +6132,7 @@
         <v>24</v>
       </c>
       <c r="B221" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C221">
         <v>1962</v>
@@ -6150,7 +6149,7 @@
         <v>230</v>
       </c>
       <c r="B222" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C222">
         <v>1962</v>
@@ -6167,7 +6166,7 @@
         <v>121</v>
       </c>
       <c r="B223" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C223">
         <v>1964</v>
@@ -6184,7 +6183,7 @@
         <v>116</v>
       </c>
       <c r="B224" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C224">
         <v>1963</v>
@@ -6201,7 +6200,7 @@
         <v>24</v>
       </c>
       <c r="B225" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C225">
         <v>1963</v>
@@ -6218,7 +6217,7 @@
         <v>24</v>
       </c>
       <c r="B226" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C226">
         <v>1963</v>
@@ -6235,7 +6234,7 @@
         <v>24</v>
       </c>
       <c r="B227" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C227">
         <v>1963</v>
@@ -6252,7 +6251,7 @@
         <v>122</v>
       </c>
       <c r="B228" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C228">
         <v>1964</v>
@@ -6269,7 +6268,7 @@
         <v>123</v>
       </c>
       <c r="B229" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C229">
         <v>1960</v>
@@ -6286,7 +6285,7 @@
         <v>24</v>
       </c>
       <c r="B230" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C230">
         <v>1964</v>
@@ -6303,7 +6302,7 @@
         <v>24</v>
       </c>
       <c r="B231" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C231">
         <v>1964</v>
@@ -6320,7 +6319,7 @@
         <v>124</v>
       </c>
       <c r="B232" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C232">
         <v>1965</v>
@@ -6334,10 +6333,10 @@
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B233" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C233">
         <v>1965</v>
@@ -6354,7 +6353,7 @@
         <v>125</v>
       </c>
       <c r="B234" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C234">
         <v>1935</v>
@@ -6371,7 +6370,7 @@
         <v>24</v>
       </c>
       <c r="B235" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C235">
         <v>1966</v>
@@ -6388,7 +6387,7 @@
         <v>24</v>
       </c>
       <c r="B236" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C236">
         <v>1967</v>
@@ -6405,7 +6404,7 @@
         <v>24</v>
       </c>
       <c r="B237" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C237">
         <v>1968</v>
@@ -6422,7 +6421,7 @@
         <v>231</v>
       </c>
       <c r="B238" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C238">
         <v>1968</v>
@@ -6439,7 +6438,7 @@
         <v>126</v>
       </c>
       <c r="B239" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C239">
         <v>1969</v>
@@ -6453,10 +6452,10 @@
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B240" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C240">
         <v>1982</v>
@@ -6473,7 +6472,7 @@
         <v>127</v>
       </c>
       <c r="B241" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C241">
         <v>1966</v>
@@ -6490,7 +6489,7 @@
         <v>128</v>
       </c>
       <c r="B242" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C242">
         <v>1970</v>
@@ -6507,7 +6506,7 @@
         <v>129</v>
       </c>
       <c r="B243" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C243">
         <v>1971</v>
@@ -6524,7 +6523,7 @@
         <v>130</v>
       </c>
       <c r="B244" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C244">
         <v>1973</v>
@@ -6558,7 +6557,7 @@
         <v>24</v>
       </c>
       <c r="B246" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C246">
         <v>1974</v>
@@ -6575,7 +6574,7 @@
         <v>24</v>
       </c>
       <c r="B247" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C247">
         <v>1974</v>
@@ -6626,7 +6625,7 @@
         <v>120</v>
       </c>
       <c r="B250" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C250">
         <v>1975</v>
@@ -6643,7 +6642,7 @@
         <v>135</v>
       </c>
       <c r="B251" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C251">
         <v>1975</v>
@@ -6660,7 +6659,7 @@
         <v>136</v>
       </c>
       <c r="B252" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C252">
         <v>1979</v>
@@ -6697,7 +6696,7 @@
         <v>138</v>
       </c>
       <c r="B254" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C254">
         <v>1980</v>
@@ -6714,7 +6713,7 @@
         <v>24</v>
       </c>
       <c r="B255" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C255">
         <v>9999</v>
@@ -6731,7 +6730,7 @@
         <v>24</v>
       </c>
       <c r="B256" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C256">
         <v>9999</v>
@@ -6748,7 +6747,7 @@
         <v>24</v>
       </c>
       <c r="B257" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C257">
         <v>9999</v>
@@ -6765,7 +6764,7 @@
         <v>24</v>
       </c>
       <c r="B258" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C258">
         <v>1983</v>
@@ -6782,7 +6781,7 @@
         <v>24</v>
       </c>
       <c r="B259" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C259">
         <v>9999</v>
@@ -6799,7 +6798,7 @@
         <v>139</v>
       </c>
       <c r="B260" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C260">
         <v>1984</v>
@@ -6816,7 +6815,7 @@
         <v>140</v>
       </c>
       <c r="B261" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C261">
         <v>1985</v>
@@ -6850,7 +6849,7 @@
         <v>143</v>
       </c>
       <c r="B263" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C263">
         <v>1987</v>
@@ -6864,10 +6863,10 @@
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B264" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C264">
         <v>1987</v>
@@ -6952,7 +6951,7 @@
         <v>150</v>
       </c>
       <c r="B269" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C269">
         <v>1835</v>
@@ -6969,7 +6968,7 @@
         <v>24</v>
       </c>
       <c r="B270" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C270">
         <v>1995</v>
@@ -7020,7 +7019,7 @@
         <v>154</v>
       </c>
       <c r="B273" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C273">
         <v>1997</v>
@@ -7057,7 +7056,7 @@
         <v>156</v>
       </c>
       <c r="B275" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C275">
         <v>1997</v>
@@ -7077,7 +7076,7 @@
         <v>157</v>
       </c>
       <c r="B276" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C276">
         <v>1998</v>
@@ -7233,7 +7232,7 @@
         <v>168</v>
       </c>
       <c r="B285" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C285">
         <v>2005</v>
@@ -7284,7 +7283,7 @@
         <v>232</v>
       </c>
       <c r="B288" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C288">
         <v>2006</v>
@@ -7406,7 +7405,7 @@
         <v>181</v>
       </c>
       <c r="B295" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C295">
         <v>2009</v>
@@ -7423,7 +7422,7 @@
         <v>24</v>
       </c>
       <c r="B296" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C296">
         <v>2010</v>
@@ -7539,10 +7538,10 @@
     </row>
     <row r="303" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
+        <v>258</v>
+      </c>
+      <c r="B303" t="s">
         <v>259</v>
-      </c>
-      <c r="B303" t="s">
-        <v>260</v>
       </c>
       <c r="C303">
         <v>2015</v>
@@ -7556,10 +7555,10 @@
     </row>
     <row r="304" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
+        <v>256</v>
+      </c>
+      <c r="B304" t="s">
         <v>257</v>
-      </c>
-      <c r="B304" t="s">
-        <v>258</v>
       </c>
       <c r="C304">
         <v>2015</v>
@@ -7576,7 +7575,7 @@
         <v>24</v>
       </c>
       <c r="B305" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C305">
         <v>2016</v>
@@ -7593,7 +7592,7 @@
         <v>24</v>
       </c>
       <c r="B306" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C306">
         <v>2017</v>
@@ -7675,13 +7674,13 @@
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>238</v>
+        <v>510</v>
       </c>
       <c r="B311" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C311">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="D311">
         <v>9999</v>

</xml_diff>